<commit_message>
reparamos bugs al abrir .csv y concatenar dframes
</commit_message>
<xml_diff>
--- a/Estacionalidad/outputs/datossss.xlsx
+++ b/Estacionalidad/outputs/datossss.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="33">
   <si>
     <t>Mes_num</t>
   </si>
@@ -470,7 +470,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:U132"/>
+  <dimension ref="A1:U133"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -600,10 +600,10 @@
         <v>4674.897526518182</v>
       </c>
       <c r="T2">
-        <v>10074.30896</v>
+        <v>295.926052</v>
       </c>
       <c r="U2">
-        <v>9320.065165506363</v>
+        <v>-29.72988752999998</v>
       </c>
     </row>
     <row r="3" spans="1:21">
@@ -665,10 +665,10 @@
         <v>4674.897526518182</v>
       </c>
       <c r="T3">
-        <v>10763.014058</v>
+        <v>35.540378</v>
       </c>
       <c r="U3">
-        <v>9320.065165506363</v>
+        <v>-29.72988752999998</v>
       </c>
     </row>
     <row r="4" spans="1:21">
@@ -730,10 +730,10 @@
         <v>4674.897526518182</v>
       </c>
       <c r="T4">
-        <v>10741.239329</v>
+        <v>24.816333</v>
       </c>
       <c r="U4">
-        <v>9320.065165506363</v>
+        <v>-29.72988752999998</v>
       </c>
     </row>
     <row r="5" spans="1:21">
@@ -795,10 +795,10 @@
         <v>4674.897526518182</v>
       </c>
       <c r="T5">
-        <v>9923.910085</v>
+        <v>-1373.317885</v>
       </c>
       <c r="U5">
-        <v>9320.065165506363</v>
+        <v>-29.72988752999998</v>
       </c>
     </row>
     <row r="6" spans="1:21">
@@ -860,10 +860,10 @@
         <v>4674.897526518182</v>
       </c>
       <c r="T6">
-        <v>8158.670578</v>
+        <v>-566.71255</v>
       </c>
       <c r="U6">
-        <v>9320.065165506363</v>
+        <v>-29.72988752999998</v>
       </c>
     </row>
     <row r="7" spans="1:21">
@@ -925,10 +925,10 @@
         <v>4674.897526518182</v>
       </c>
       <c r="T7">
-        <v>8004.148869</v>
+        <v>-242.369417</v>
       </c>
       <c r="U7">
-        <v>9320.065165506363</v>
+        <v>-29.72988752999998</v>
       </c>
     </row>
     <row r="8" spans="1:21">
@@ -990,10 +990,10 @@
         <v>4674.897526518182</v>
       </c>
       <c r="T8">
-        <v>8634.871404040001</v>
+        <v>-53.36128815999999</v>
       </c>
       <c r="U8">
-        <v>9320.065165506363</v>
+        <v>-29.72988752999998</v>
       </c>
     </row>
     <row r="9" spans="1:21">
@@ -1055,10 +1055,10 @@
         <v>4674.897526518182</v>
       </c>
       <c r="T9">
-        <v>10553.5043025</v>
+        <v>-933.02353878</v>
       </c>
       <c r="U9">
-        <v>9320.065165506363</v>
+        <v>-29.72988752999998</v>
       </c>
     </row>
     <row r="10" spans="1:21">
@@ -1120,10 +1120,10 @@
         <v>4674.897526518182</v>
       </c>
       <c r="T10">
-        <v>8796.59928495</v>
+        <v>372.98567283</v>
       </c>
       <c r="U10">
-        <v>9320.065165506363</v>
+        <v>-29.72988752999998</v>
       </c>
     </row>
     <row r="11" spans="1:21">
@@ -1185,10 +1185,10 @@
         <v>4674.897526518182</v>
       </c>
       <c r="T11">
-        <v>8114.902665109999</v>
+        <v>1044.03497147</v>
       </c>
       <c r="U11">
-        <v>9320.065165506363</v>
+        <v>-29.72988752999998</v>
       </c>
     </row>
     <row r="12" spans="1:21">
@@ -1250,10 +1250,10 @@
         <v>4674.897526518182</v>
       </c>
       <c r="T12">
-        <v>8755.54728497</v>
+        <v>1068.45250881</v>
       </c>
       <c r="U12">
-        <v>9320.065165506363</v>
+        <v>-29.72988752999998</v>
       </c>
     </row>
     <row r="13" spans="1:21">
@@ -1315,10 +1315,10 @@
         <v>4417.916156005454</v>
       </c>
       <c r="T13">
-        <v>10162.295412</v>
+        <v>633.739044</v>
       </c>
       <c r="U13">
-        <v>9033.638398951818</v>
+        <v>197.8060869409091</v>
       </c>
     </row>
     <row r="14" spans="1:21">
@@ -1380,10 +1380,10 @@
         <v>4417.916156005454</v>
       </c>
       <c r="T14">
-        <v>10729.493607</v>
+        <v>1279.552631</v>
       </c>
       <c r="U14">
-        <v>9033.638398951818</v>
+        <v>197.8060869409091</v>
       </c>
     </row>
     <row r="15" spans="1:21">
@@ -1445,10 +1445,10 @@
         <v>4417.916156005454</v>
       </c>
       <c r="T15">
-        <v>10080.603395</v>
+        <v>-268.866931</v>
       </c>
       <c r="U15">
-        <v>9033.638398951818</v>
+        <v>197.8060869409091</v>
       </c>
     </row>
     <row r="16" spans="1:21">
@@ -1510,10 +1510,10 @@
         <v>4417.916156005454</v>
       </c>
       <c r="T16">
-        <v>10185.168357</v>
+        <v>-889.714355</v>
       </c>
       <c r="U16">
-        <v>9033.638398951818</v>
+        <v>197.8060869409091</v>
       </c>
     </row>
     <row r="17" spans="1:21">
@@ -1575,10 +1575,10 @@
         <v>4417.916156005454</v>
       </c>
       <c r="T17">
-        <v>7956.200829</v>
+        <v>-212.776157</v>
       </c>
       <c r="U17">
-        <v>9033.638398951818</v>
+        <v>197.8060869409091</v>
       </c>
     </row>
     <row r="18" spans="1:21">
@@ -1640,10 +1640,10 @@
         <v>4417.916156005454</v>
       </c>
       <c r="T18">
-        <v>8237.073343</v>
+        <v>44.719567</v>
       </c>
       <c r="U18">
-        <v>9033.638398951818</v>
+        <v>197.8060869409091</v>
       </c>
     </row>
     <row r="19" spans="1:21">
@@ -1705,10 +1705,10 @@
         <v>4417.916156005454</v>
       </c>
       <c r="T19">
-        <v>8016.51639449</v>
+        <v>-217.82092465</v>
       </c>
       <c r="U19">
-        <v>9033.638398951818</v>
+        <v>197.8060869409091</v>
       </c>
     </row>
     <row r="20" spans="1:21">
@@ -1770,10 +1770,10 @@
         <v>4417.916156005454</v>
       </c>
       <c r="T20">
-        <v>9500.194216129999</v>
+        <v>-891.76621721</v>
       </c>
       <c r="U20">
-        <v>9033.638398951818</v>
+        <v>197.8060869409091</v>
       </c>
     </row>
     <row r="21" spans="1:21">
@@ -1835,10 +1835,10 @@
         <v>4417.916156005454</v>
       </c>
       <c r="T21">
-        <v>8445.590784850001</v>
+        <v>449.71589261</v>
       </c>
       <c r="U21">
-        <v>9033.638398951818</v>
+        <v>197.8060869409091</v>
       </c>
     </row>
     <row r="22" spans="1:21">
@@ -1900,10 +1900,10 @@
         <v>4417.916156005454</v>
       </c>
       <c r="T22">
-        <v>7569.21046097</v>
+        <v>1186.76200589</v>
       </c>
       <c r="U22">
-        <v>9033.638398951818</v>
+        <v>197.8060869409091</v>
       </c>
     </row>
     <row r="23" spans="1:21">
@@ -1965,10 +1965,10 @@
         <v>4417.916156005454</v>
       </c>
       <c r="T23">
-        <v>8487.675589029999</v>
+        <v>1062.32240071</v>
       </c>
       <c r="U23">
-        <v>9033.638398951818</v>
+        <v>197.8060869409091</v>
       </c>
     </row>
     <row r="24" spans="1:21">
@@ -2030,10 +2030,10 @@
         <v>5026.986619191818</v>
       </c>
       <c r="T24">
-        <v>11739.679625</v>
+        <v>456.524457</v>
       </c>
       <c r="U24">
-        <v>10244.64484361273</v>
+        <v>190.6716052290909</v>
       </c>
     </row>
     <row r="25" spans="1:21">
@@ -2095,10 +2095,10 @@
         <v>5026.986619191818</v>
       </c>
       <c r="T25">
-        <v>11346.462122</v>
+        <v>1053.469376</v>
       </c>
       <c r="U25">
-        <v>10244.64484361273</v>
+        <v>190.6716052290909</v>
       </c>
     </row>
     <row r="26" spans="1:21">
@@ -2160,10 +2160,10 @@
         <v>5026.986619191818</v>
       </c>
       <c r="T26">
-        <v>11779.110597</v>
+        <v>540.779253</v>
       </c>
       <c r="U26">
-        <v>10244.64484361273</v>
+        <v>190.6716052290909</v>
       </c>
     </row>
     <row r="27" spans="1:21">
@@ -2225,10 +2225,10 @@
         <v>5026.986619191818</v>
       </c>
       <c r="T27">
-        <v>10302.830162</v>
+        <v>-476.926572</v>
       </c>
       <c r="U27">
-        <v>10244.64484361273</v>
+        <v>190.6716052290909</v>
       </c>
     </row>
     <row r="28" spans="1:21">
@@ -2290,10 +2290,10 @@
         <v>5026.986619191818</v>
       </c>
       <c r="T28">
-        <v>9440.263077</v>
+        <v>-677.352243</v>
       </c>
       <c r="U28">
-        <v>10244.64484361273</v>
+        <v>190.6716052290909</v>
       </c>
     </row>
     <row r="29" spans="1:21">
@@ -2355,10 +2355,10 @@
         <v>5026.986619191818</v>
       </c>
       <c r="T29">
-        <v>8977.166373</v>
+        <v>-135.477555</v>
       </c>
       <c r="U29">
-        <v>10244.64484361273</v>
+        <v>190.6716052290909</v>
       </c>
     </row>
     <row r="30" spans="1:21">
@@ -2420,10 +2420,10 @@
         <v>5026.986619191818</v>
       </c>
       <c r="T30">
-        <v>10039.65441606</v>
+        <v>-910.31219326</v>
       </c>
       <c r="U30">
-        <v>10244.64484361273</v>
+        <v>190.6716052290909</v>
       </c>
     </row>
     <row r="31" spans="1:21">
@@ -2485,10 +2485,10 @@
         <v>5026.986619191818</v>
       </c>
       <c r="T31">
-        <v>11395.61447384</v>
+        <v>-562.2848089600001</v>
       </c>
       <c r="U31">
-        <v>10244.64484361273</v>
+        <v>190.6716052290909</v>
       </c>
     </row>
     <row r="32" spans="1:21">
@@ -2550,10 +2550,10 @@
         <v>5026.986619191818</v>
       </c>
       <c r="T32">
-        <v>9093.28474347</v>
+        <v>1180.65928273</v>
       </c>
       <c r="U32">
-        <v>10244.64484361273</v>
+        <v>190.6716052290909</v>
       </c>
     </row>
     <row r="33" spans="1:21">
@@ -2615,10 +2615,10 @@
         <v>5026.986619191818</v>
       </c>
       <c r="T33">
-        <v>7536.85732592</v>
+        <v>1228.48143192</v>
       </c>
       <c r="U33">
-        <v>10244.64484361273</v>
+        <v>190.6716052290909</v>
       </c>
     </row>
     <row r="34" spans="1:21">
@@ -2680,10 +2680,10 @@
         <v>5026.986619191818</v>
       </c>
       <c r="T34">
-        <v>11040.17036445</v>
+        <v>399.8272290899999</v>
       </c>
       <c r="U34">
-        <v>10244.64484361273</v>
+        <v>190.6716052290909</v>
       </c>
     </row>
     <row r="35" spans="1:21">
@@ -2745,10 +2745,10 @@
         <v>4938.730177490909</v>
       </c>
       <c r="T35">
-        <v>12575.753152</v>
+        <v>1509.978876</v>
       </c>
       <c r="U35">
-        <v>10660.45371784</v>
+        <v>782.9933628581817</v>
       </c>
     </row>
     <row r="36" spans="1:21">
@@ -2810,10 +2810,10 @@
         <v>4938.730177490909</v>
       </c>
       <c r="T36">
-        <v>11484.751018</v>
+        <v>1945.149404</v>
       </c>
       <c r="U36">
-        <v>10660.45371784</v>
+        <v>782.9933628581817</v>
       </c>
     </row>
     <row r="37" spans="1:21">
@@ -2875,10 +2875,10 @@
         <v>4938.730177490909</v>
       </c>
       <c r="T37">
-        <v>13088.82901</v>
+        <v>701.94122</v>
       </c>
       <c r="U37">
-        <v>10660.45371784</v>
+        <v>782.9933628581817</v>
       </c>
     </row>
     <row r="38" spans="1:21">
@@ -2940,10 +2940,10 @@
         <v>4938.730177490909</v>
       </c>
       <c r="T38">
-        <v>12134.643422</v>
+        <v>822.39112</v>
       </c>
       <c r="U38">
-        <v>10660.45371784</v>
+        <v>782.9933628581817</v>
       </c>
     </row>
     <row r="39" spans="1:21">
@@ -3005,10 +3005,10 @@
         <v>4938.730177490909</v>
       </c>
       <c r="T39">
-        <v>10088.202538</v>
+        <v>222.33081</v>
       </c>
       <c r="U39">
-        <v>10660.45371784</v>
+        <v>782.9933628581817</v>
       </c>
     </row>
     <row r="40" spans="1:21">
@@ -3070,10 +3070,10 @@
         <v>4938.730177490909</v>
       </c>
       <c r="T40">
-        <v>9162.19491</v>
+        <v>316.909954</v>
       </c>
       <c r="U40">
-        <v>10660.45371784</v>
+        <v>782.9933628581817</v>
       </c>
     </row>
     <row r="41" spans="1:21">
@@ -3135,10 +3135,10 @@
         <v>4938.730177490909</v>
       </c>
       <c r="T41">
-        <v>9839.73226805</v>
+        <v>-106.47264349</v>
       </c>
       <c r="U41">
-        <v>10660.45371784</v>
+        <v>782.9933628581817</v>
       </c>
     </row>
     <row r="42" spans="1:21">
@@ -3200,10 +3200,10 @@
         <v>4938.730177490909</v>
       </c>
       <c r="T42">
-        <v>11321.91600667</v>
+        <v>-889.25412339</v>
       </c>
       <c r="U42">
-        <v>10660.45371784</v>
+        <v>782.9933628581817</v>
       </c>
     </row>
     <row r="43" spans="1:21">
@@ -3265,10 +3265,10 @@
         <v>4938.730177490909</v>
       </c>
       <c r="T43">
-        <v>9509.45708115</v>
+        <v>1164.89381463</v>
       </c>
       <c r="U43">
-        <v>10660.45371784</v>
+        <v>782.9933628581817</v>
       </c>
     </row>
     <row r="44" spans="1:21">
@@ -3330,10 +3330,10 @@
         <v>4938.730177490909</v>
       </c>
       <c r="T44">
-        <v>7243.70565972</v>
+        <v>1454.86699044</v>
       </c>
       <c r="U44">
-        <v>10660.45371784</v>
+        <v>782.9933628581817</v>
       </c>
     </row>
     <row r="45" spans="1:21">
@@ -3395,10 +3395,10 @@
         <v>4938.730177490909</v>
       </c>
       <c r="T45">
-        <v>10815.80583065</v>
+        <v>1470.19156925</v>
       </c>
       <c r="U45">
-        <v>10660.45371784</v>
+        <v>782.9933628581817</v>
       </c>
     </row>
     <row r="46" spans="1:21">
@@ -3460,10 +3460,10 @@
         <v>5511.125900494546</v>
       </c>
       <c r="T46">
-        <v>14422.691015</v>
+        <v>1443.051581</v>
       </c>
       <c r="U46">
-        <v>11853.37480181</v>
+        <v>831.1230008209092</v>
       </c>
     </row>
     <row r="47" spans="1:21">
@@ -3525,10 +3525,10 @@
         <v>5511.125900494546</v>
       </c>
       <c r="T47">
-        <v>13067.90971</v>
+        <v>1093.734298</v>
       </c>
       <c r="U47">
-        <v>11853.37480181</v>
+        <v>831.1230008209092</v>
       </c>
     </row>
     <row r="48" spans="1:21">
@@ -3590,10 +3590,10 @@
         <v>5511.125900494546</v>
       </c>
       <c r="T48">
-        <v>15421.314263</v>
+        <v>1365.164707</v>
       </c>
       <c r="U48">
-        <v>11853.37480181</v>
+        <v>831.1230008209092</v>
       </c>
     </row>
     <row r="49" spans="1:21">
@@ -3655,10 +3655,10 @@
         <v>5511.125900494546</v>
       </c>
       <c r="T49">
-        <v>12955.418161</v>
+        <v>1401.606939</v>
       </c>
       <c r="U49">
-        <v>11853.37480181</v>
+        <v>831.1230008209092</v>
       </c>
     </row>
     <row r="50" spans="1:21">
@@ -3720,10 +3720,10 @@
         <v>5511.125900494546</v>
       </c>
       <c r="T50">
-        <v>10208.389334</v>
+        <v>202.609028</v>
       </c>
       <c r="U50">
-        <v>11853.37480181</v>
+        <v>831.1230008209092</v>
       </c>
     </row>
     <row r="51" spans="1:21">
@@ -3785,10 +3785,10 @@
         <v>5511.125900494546</v>
       </c>
       <c r="T51">
-        <v>10256.993675</v>
+        <v>509.859325</v>
       </c>
       <c r="U51">
-        <v>11853.37480181</v>
+        <v>831.1230008209092</v>
       </c>
     </row>
     <row r="52" spans="1:21">
@@ -3850,10 +3850,10 @@
         <v>5511.125900494546</v>
       </c>
       <c r="T52">
-        <v>11557.50222713</v>
+        <v>-571.1389577699999</v>
       </c>
       <c r="U52">
-        <v>11853.37480181</v>
+        <v>831.1230008209092</v>
       </c>
     </row>
     <row r="53" spans="1:21">
@@ -3915,10 +3915,10 @@
         <v>5511.125900494546</v>
       </c>
       <c r="T53">
-        <v>11611.05576323</v>
+        <v>-1284.94533607</v>
       </c>
       <c r="U53">
-        <v>11853.37480181</v>
+        <v>831.1230008209092</v>
       </c>
     </row>
     <row r="54" spans="1:21">
@@ -3980,10 +3980,10 @@
         <v>5511.125900494546</v>
       </c>
       <c r="T54">
-        <v>10688.47862992</v>
+        <v>1398.90118706</v>
       </c>
       <c r="U54">
-        <v>11853.37480181</v>
+        <v>831.1230008209092</v>
       </c>
     </row>
     <row r="55" spans="1:21">
@@ -4045,10 +4045,10 @@
         <v>5511.125900494546</v>
       </c>
       <c r="T55">
-        <v>8243.677177080001</v>
+        <v>1911.82067988</v>
       </c>
       <c r="U55">
-        <v>11853.37480181</v>
+        <v>831.1230008209092</v>
       </c>
     </row>
     <row r="56" spans="1:21">
@@ -4110,10 +4110,10 @@
         <v>5511.125900494546</v>
       </c>
       <c r="T56">
-        <v>11953.69286455</v>
+        <v>1671.68955793</v>
       </c>
       <c r="U56">
-        <v>11853.37480181</v>
+        <v>831.1230008209092</v>
       </c>
     </row>
     <row r="57" spans="1:21">
@@ -4175,10 +4175,10 @@
         <v>5520.058835477273</v>
       </c>
       <c r="T57">
-        <v>14521.504263</v>
+        <v>1112.434651</v>
       </c>
       <c r="U57">
-        <v>11702.28440521818</v>
+        <v>662.1667342636364</v>
       </c>
     </row>
     <row r="58" spans="1:21">
@@ -4240,10 +4240,10 @@
         <v>5520.058835477273</v>
       </c>
       <c r="T58">
-        <v>12855.656127</v>
+        <v>788.673489</v>
       </c>
       <c r="U58">
-        <v>11702.28440521818</v>
+        <v>662.1667342636364</v>
       </c>
     </row>
     <row r="59" spans="1:21">
@@ -4305,10 +4305,10 @@
         <v>5520.058835477273</v>
       </c>
       <c r="T59">
-        <v>14126.179833</v>
+        <v>840.595273</v>
       </c>
       <c r="U59">
-        <v>11702.28440521818</v>
+        <v>662.1667342636364</v>
       </c>
     </row>
     <row r="60" spans="1:21">
@@ -4370,10 +4370,10 @@
         <v>5520.058835477273</v>
       </c>
       <c r="T60">
-        <v>13051.47131</v>
+        <v>1355.931494</v>
       </c>
       <c r="U60">
-        <v>11702.28440521818</v>
+        <v>662.1667342636364</v>
       </c>
     </row>
     <row r="61" spans="1:21">
@@ -4435,10 +4435,10 @@
         <v>5520.058835477273</v>
       </c>
       <c r="T61">
-        <v>11753.520875</v>
+        <v>339.416761</v>
       </c>
       <c r="U61">
-        <v>11702.28440521818</v>
+        <v>662.1667342636364</v>
       </c>
     </row>
     <row r="62" spans="1:21">
@@ -4500,10 +4500,10 @@
         <v>5520.058835477273</v>
       </c>
       <c r="T62">
-        <v>10351.289939</v>
+        <v>258.571999</v>
       </c>
       <c r="U62">
-        <v>11702.28440521818</v>
+        <v>662.1667342636364</v>
       </c>
     </row>
     <row r="63" spans="1:21">
@@ -4565,10 +4565,10 @@
         <v>5520.058835477273</v>
       </c>
       <c r="T63">
-        <v>11056.63501634</v>
+        <v>-739.66141304</v>
       </c>
       <c r="U63">
-        <v>11702.28440521818</v>
+        <v>662.1667342636364</v>
       </c>
     </row>
     <row r="64" spans="1:21">
@@ -4630,10 +4630,10 @@
         <v>5520.058835477273</v>
       </c>
       <c r="T64">
-        <v>10594.44543924</v>
+        <v>-327.59327862</v>
       </c>
       <c r="U64">
-        <v>11702.28440521818</v>
+        <v>662.1667342636364</v>
       </c>
     </row>
     <row r="65" spans="1:21">
@@ -4695,10 +4695,10 @@
         <v>5520.058835477273</v>
       </c>
       <c r="T65">
-        <v>9410.536738569999</v>
+        <v>1067.75312755</v>
       </c>
       <c r="U65">
-        <v>11702.28440521818</v>
+        <v>662.1667342636364</v>
       </c>
     </row>
     <row r="66" spans="1:21">
@@ -4760,10 +4760,10 @@
         <v>5520.058835477273</v>
       </c>
       <c r="T66">
-        <v>8085.253705810001</v>
+        <v>1486.63970807</v>
       </c>
       <c r="U66">
-        <v>11702.28440521818</v>
+        <v>662.1667342636364</v>
       </c>
     </row>
     <row r="67" spans="1:21">
@@ -4825,10 +4825,10 @@
         <v>5520.058835477273</v>
       </c>
       <c r="T67">
-        <v>12918.63521044</v>
+        <v>1101.07226594</v>
       </c>
       <c r="U67">
-        <v>11702.28440521818</v>
+        <v>662.1667342636364</v>
       </c>
     </row>
     <row r="68" spans="1:21">
@@ -4890,10 +4890,10 @@
         <v>5741.041278345455</v>
       </c>
       <c r="T68">
-        <v>14084.127172</v>
+        <v>367.068636</v>
       </c>
       <c r="U68">
-        <v>11882.52766401</v>
+        <v>400.4451073190909</v>
       </c>
     </row>
     <row r="69" spans="1:21">
@@ -4955,10 +4955,10 @@
         <v>5741.041278345455</v>
       </c>
       <c r="T69">
-        <v>13999.972101</v>
+        <v>1310.245357</v>
       </c>
       <c r="U69">
-        <v>11882.52766401</v>
+        <v>400.4451073190909</v>
       </c>
     </row>
     <row r="70" spans="1:21">
@@ -5020,10 +5020,10 @@
         <v>5741.041278345455</v>
       </c>
       <c r="T70">
-        <v>13918.792099</v>
+        <v>-57.489841</v>
       </c>
       <c r="U70">
-        <v>11882.52766401</v>
+        <v>400.4451073190909</v>
       </c>
     </row>
     <row r="71" spans="1:21">
@@ -5085,10 +5085,10 @@
         <v>5741.041278345455</v>
       </c>
       <c r="T71">
-        <v>12561.980209</v>
+        <v>271.836663</v>
       </c>
       <c r="U71">
-        <v>11882.52766401</v>
+        <v>400.4451073190909</v>
       </c>
     </row>
     <row r="72" spans="1:21">
@@ -5150,10 +5150,10 @@
         <v>5741.041278345455</v>
       </c>
       <c r="T72">
-        <v>11369.451414</v>
+        <v>-231.674068</v>
       </c>
       <c r="U72">
-        <v>11882.52766401</v>
+        <v>400.4451073190909</v>
       </c>
     </row>
     <row r="73" spans="1:21">
@@ -5215,10 +5215,10 @@
         <v>5741.041278345455</v>
       </c>
       <c r="T73">
-        <v>9719.225692</v>
+        <v>283.97967</v>
       </c>
       <c r="U73">
-        <v>11882.52766401</v>
+        <v>400.4451073190909</v>
       </c>
     </row>
     <row r="74" spans="1:21">
@@ -5280,10 +5280,10 @@
         <v>5741.041278345455</v>
       </c>
       <c r="T74">
-        <v>11346.81979467</v>
+        <v>-738.65249357</v>
       </c>
       <c r="U74">
-        <v>11882.52766401</v>
+        <v>400.4451073190909</v>
       </c>
     </row>
     <row r="75" spans="1:21">
@@ -5345,10 +5345,10 @@
         <v>5741.041278345455</v>
       </c>
       <c r="T75">
-        <v>11597.2320744</v>
+        <v>-767.56997356</v>
       </c>
       <c r="U75">
-        <v>11882.52766401</v>
+        <v>400.4451073190909</v>
       </c>
     </row>
     <row r="76" spans="1:21">
@@ -5410,10 +5410,10 @@
         <v>5741.041278345455</v>
       </c>
       <c r="T76">
-        <v>10761.01430881</v>
+        <v>950.41862725</v>
       </c>
       <c r="U76">
-        <v>11882.52766401</v>
+        <v>400.4451073190909</v>
       </c>
     </row>
     <row r="77" spans="1:21">
@@ -5475,10 +5475,10 @@
         <v>5741.041278345455</v>
       </c>
       <c r="T77">
-        <v>8381.84412836</v>
+        <v>1480.2650479</v>
       </c>
       <c r="U77">
-        <v>11882.52766401</v>
+        <v>400.4451073190909</v>
       </c>
     </row>
     <row r="78" spans="1:21">
@@ -5540,10 +5540,10 @@
         <v>5741.041278345455</v>
       </c>
       <c r="T78">
-        <v>12967.34531087</v>
+        <v>1536.46855549</v>
       </c>
       <c r="U78">
-        <v>11882.52766401</v>
+        <v>400.4451073190909</v>
       </c>
     </row>
     <row r="79" spans="1:21">
@@ -5605,10 +5605,10 @@
         <v>5794.301558027273</v>
       </c>
       <c r="T79">
-        <v>15999.498435</v>
+        <v>657.410995</v>
       </c>
       <c r="U79">
-        <v>12102.86625686727</v>
+        <v>514.2631408127273</v>
       </c>
     </row>
     <row r="80" spans="1:21">
@@ -5670,10 +5670,10 @@
         <v>5794.301558027273</v>
       </c>
       <c r="T80">
-        <v>13727.515192</v>
+        <v>1174.678624</v>
       </c>
       <c r="U80">
-        <v>12102.86625686727</v>
+        <v>514.2631408127273</v>
       </c>
     </row>
     <row r="81" spans="1:21">
@@ -5735,10 +5735,10 @@
         <v>5794.301558027273</v>
       </c>
       <c r="T81">
-        <v>14273.415172</v>
+        <v>125.647118</v>
       </c>
       <c r="U81">
-        <v>12102.86625686727</v>
+        <v>514.2631408127273</v>
       </c>
     </row>
     <row r="82" spans="1:21">
@@ -5800,10 +5800,10 @@
         <v>5794.301558027273</v>
       </c>
       <c r="T82">
-        <v>12064.324689</v>
+        <v>775.575831</v>
       </c>
       <c r="U82">
-        <v>12102.86625686727</v>
+        <v>514.2631408127273</v>
       </c>
     </row>
     <row r="83" spans="1:21">
@@ -5865,10 +5865,10 @@
         <v>5794.301558027273</v>
       </c>
       <c r="T83">
-        <v>10740.652527</v>
+        <v>-469.213959</v>
       </c>
       <c r="U83">
-        <v>12102.86625686727</v>
+        <v>514.2631408127273</v>
       </c>
     </row>
     <row r="84" spans="1:21">
@@ -5930,10 +5930,10 @@
         <v>5794.301558027273</v>
       </c>
       <c r="T84">
-        <v>10937.443018</v>
+        <v>590.0863880000001</v>
       </c>
       <c r="U84">
-        <v>12102.86625686727</v>
+        <v>514.2631408127273</v>
       </c>
     </row>
     <row r="85" spans="1:21">
@@ -5995,10 +5995,10 @@
         <v>5794.301558027273</v>
       </c>
       <c r="T85">
-        <v>11589.10915705</v>
+        <v>-1044.35476557</v>
       </c>
       <c r="U85">
-        <v>12102.86625686727</v>
+        <v>514.2631408127273</v>
       </c>
     </row>
     <row r="86" spans="1:21">
@@ -6060,10 +6060,10 @@
         <v>5794.301558027273</v>
       </c>
       <c r="T86">
-        <v>11516.11117799</v>
+        <v>-1112.49082807</v>
       </c>
       <c r="U86">
-        <v>12102.86625686727</v>
+        <v>514.2631408127273</v>
       </c>
     </row>
     <row r="87" spans="1:21">
@@ -6125,10 +6125,10 @@
         <v>5794.301558027273</v>
       </c>
       <c r="T87">
-        <v>9968.129817120001</v>
+        <v>1167.9414548</v>
       </c>
       <c r="U87">
-        <v>12102.86625686727</v>
+        <v>514.2631408127273</v>
       </c>
     </row>
     <row r="88" spans="1:21">
@@ -6190,10 +6190,10 @@
         <v>5794.301558027273</v>
       </c>
       <c r="T88">
-        <v>8462.829420030001</v>
+        <v>1446.40144717</v>
       </c>
       <c r="U88">
-        <v>12102.86625686727</v>
+        <v>514.2631408127273</v>
       </c>
     </row>
     <row r="89" spans="1:21">
@@ -6255,10 +6255,10 @@
         <v>5794.301558027273</v>
       </c>
       <c r="T89">
-        <v>13852.50022035</v>
+        <v>2345.21224361</v>
       </c>
       <c r="U89">
-        <v>12102.86625686727</v>
+        <v>514.2631408127273</v>
       </c>
     </row>
     <row r="90" spans="1:21">
@@ -6320,10 +6320,10 @@
         <v>5393.591845370909</v>
       </c>
       <c r="T90">
-        <v>14606.688451</v>
+        <v>829.693903</v>
       </c>
       <c r="U90">
-        <v>11330.92436248636</v>
+        <v>543.7406717445455</v>
       </c>
     </row>
     <row r="91" spans="1:21">
@@ -6385,10 +6385,10 @@
         <v>5393.591845370909</v>
       </c>
       <c r="T91">
-        <v>12657.735242</v>
+        <v>948.508268</v>
       </c>
       <c r="U91">
-        <v>11330.92436248636</v>
+        <v>543.7406717445455</v>
       </c>
     </row>
     <row r="92" spans="1:21">
@@ -6450,10 +6450,10 @@
         <v>5393.591845370909</v>
       </c>
       <c r="T92">
-        <v>12573.719763</v>
+        <v>515.883809</v>
       </c>
       <c r="U92">
-        <v>11330.92436248636</v>
+        <v>543.7406717445455</v>
       </c>
     </row>
     <row r="93" spans="1:21">
@@ -6515,10 +6515,10 @@
         <v>5393.591845370909</v>
       </c>
       <c r="T93">
-        <v>11329.301244</v>
+        <v>41.152776</v>
       </c>
       <c r="U93">
-        <v>11330.92436248636</v>
+        <v>543.7406717445455</v>
       </c>
     </row>
     <row r="94" spans="1:21">
@@ -6580,10 +6580,10 @@
         <v>5393.591845370909</v>
       </c>
       <c r="T94">
-        <v>10649.072014</v>
+        <v>-325.077078</v>
       </c>
       <c r="U94">
-        <v>11330.92436248636</v>
+        <v>543.7406717445455</v>
       </c>
     </row>
     <row r="95" spans="1:21">
@@ -6645,10 +6645,10 @@
         <v>5393.591845370909</v>
       </c>
       <c r="T95">
-        <v>9790.958619999999</v>
+        <v>308.133574</v>
       </c>
       <c r="U95">
-        <v>11330.92436248636</v>
+        <v>543.7406717445455</v>
       </c>
     </row>
     <row r="96" spans="1:21">
@@ -6710,10 +6710,10 @@
         <v>5393.591845370909</v>
       </c>
       <c r="T96">
-        <v>11236.58452193</v>
+        <v>-700.1108071900001</v>
       </c>
       <c r="U96">
-        <v>11330.92436248636</v>
+        <v>543.7406717445455</v>
       </c>
     </row>
     <row r="97" spans="1:21">
@@ -6775,10 +6775,10 @@
         <v>5393.591845370909</v>
       </c>
       <c r="T97">
-        <v>9736.763026299999</v>
+        <v>336.85376734</v>
       </c>
       <c r="U97">
-        <v>11330.92436248636</v>
+        <v>543.7406717445455</v>
       </c>
     </row>
     <row r="98" spans="1:21">
@@ -6840,10 +6840,10 @@
         <v>5393.591845370909</v>
       </c>
       <c r="T98">
-        <v>9747.97882041</v>
+        <v>1744.09521031</v>
       </c>
       <c r="U98">
-        <v>11330.92436248636</v>
+        <v>543.7406717445455</v>
       </c>
     </row>
     <row r="99" spans="1:21">
@@ -6905,10 +6905,10 @@
         <v>5393.591845370909</v>
       </c>
       <c r="T99">
-        <v>8855.494942860001</v>
+        <v>597.5067277000001</v>
       </c>
       <c r="U99">
-        <v>11330.92436248636</v>
+        <v>543.7406717445455</v>
       </c>
     </row>
     <row r="100" spans="1:21">
@@ -6970,10 +6970,10 @@
         <v>5393.591845370909</v>
       </c>
       <c r="T100">
-        <v>13455.87134185</v>
+        <v>1684.50723903</v>
       </c>
       <c r="U100">
-        <v>11330.92436248636</v>
+        <v>543.7406717445455</v>
       </c>
     </row>
     <row r="101" spans="1:21">
@@ -7035,10 +7035,10 @@
         <v>5398.313126614546</v>
       </c>
       <c r="T101">
-        <v>13738.411494</v>
+        <v>1132.411662</v>
       </c>
       <c r="U101">
-        <v>11218.28270152546</v>
+        <v>421.6564482963637</v>
       </c>
     </row>
     <row r="102" spans="1:21">
@@ -7100,10 +7100,10 @@
         <v>5398.313126614546</v>
       </c>
       <c r="T102">
-        <v>13145.80064</v>
+        <v>632.6058860000001</v>
       </c>
       <c r="U102">
-        <v>11218.28270152546</v>
+        <v>421.6564482963637</v>
       </c>
     </row>
     <row r="103" spans="1:21">
@@ -7165,10 +7165,10 @@
         <v>5398.313126614546</v>
       </c>
       <c r="T103">
-        <v>12857.914525</v>
+        <v>-803.9730510000001</v>
       </c>
       <c r="U103">
-        <v>11218.28270152546</v>
+        <v>421.6564482963637</v>
       </c>
     </row>
     <row r="104" spans="1:21">
@@ -7230,10 +7230,10 @@
         <v>5398.313126614546</v>
       </c>
       <c r="T104">
-        <v>11288.297856</v>
+        <v>299.766384</v>
       </c>
       <c r="U104">
-        <v>11218.28270152546</v>
+        <v>421.6564482963637</v>
       </c>
     </row>
     <row r="105" spans="1:21">
@@ -7295,10 +7295,10 @@
         <v>5398.313126614546</v>
       </c>
       <c r="T105">
-        <v>10090.939058</v>
+        <v>-25.034368</v>
       </c>
       <c r="U105">
-        <v>11218.28270152546</v>
+        <v>421.6564482963637</v>
       </c>
     </row>
     <row r="106" spans="1:21">
@@ -7360,10 +7360,10 @@
         <v>5398.313126614546</v>
       </c>
       <c r="T106">
-        <v>9519.668879999999</v>
+        <v>-46.210702</v>
       </c>
       <c r="U106">
-        <v>11218.28270152546</v>
+        <v>421.6564482963637</v>
       </c>
     </row>
     <row r="107" spans="1:21">
@@ -7425,10 +7425,10 @@
         <v>5398.313126614546</v>
       </c>
       <c r="T107">
-        <v>11489.66733358</v>
+        <v>-928.60080272</v>
       </c>
       <c r="U107">
-        <v>11218.28270152546</v>
+        <v>421.6564482963637</v>
       </c>
     </row>
     <row r="108" spans="1:21">
@@ -7490,10 +7490,10 @@
         <v>5398.313126614546</v>
       </c>
       <c r="T108">
-        <v>10471.59927549</v>
+        <v>324.65191189</v>
       </c>
       <c r="U108">
-        <v>11218.28270152546</v>
+        <v>421.6564482963637</v>
       </c>
     </row>
     <row r="109" spans="1:21">
@@ -7555,10 +7555,10 @@
         <v>5398.313126614546</v>
       </c>
       <c r="T109">
-        <v>10010.52303408</v>
+        <v>1767.66255324</v>
       </c>
       <c r="U109">
-        <v>11218.28270152546</v>
+        <v>421.6564482963637</v>
       </c>
     </row>
     <row r="110" spans="1:21">
@@ -7620,10 +7620,10 @@
         <v>5398.313126614546</v>
       </c>
       <c r="T110">
-        <v>8678.4853871</v>
+        <v>669.60349684</v>
       </c>
       <c r="U110">
-        <v>11218.28270152546</v>
+        <v>421.6564482963637</v>
       </c>
     </row>
     <row r="111" spans="1:21">
@@ -7685,10 +7685,10 @@
         <v>5398.313126614546</v>
       </c>
       <c r="T111">
-        <v>12109.80223353</v>
+        <v>1615.33796101</v>
       </c>
       <c r="U111">
-        <v>11218.28270152546</v>
+        <v>421.6564482963637</v>
       </c>
     </row>
     <row r="112" spans="1:21">
@@ -7741,19 +7741,19 @@
         <v>6493.159464</v>
       </c>
       <c r="Q112">
-        <v>5321.098394290909</v>
+        <v>5323.552942100909</v>
       </c>
       <c r="R112">
         <v>6229.740888</v>
       </c>
       <c r="S112">
-        <v>5090.122174681818</v>
+        <v>5089.209807263636</v>
       </c>
       <c r="T112">
-        <v>12722.900352</v>
+        <v>263.418576</v>
       </c>
       <c r="U112">
-        <v>10411.22056897273</v>
+        <v>1281.070407564545</v>
       </c>
     </row>
     <row r="113" spans="1:21">
@@ -7806,19 +7806,19 @@
         <v>6649.420587</v>
       </c>
       <c r="Q113">
-        <v>5321.098394290909</v>
+        <v>5323.552942100909</v>
       </c>
       <c r="R113">
         <v>5779.456393</v>
       </c>
       <c r="S113">
-        <v>5090.122174681818</v>
+        <v>5089.209807263636</v>
       </c>
       <c r="T113">
-        <v>12428.87698</v>
+        <v>869.964194</v>
       </c>
       <c r="U113">
-        <v>10411.22056897273</v>
+        <v>1281.070407564545</v>
       </c>
     </row>
     <row r="114" spans="1:21">
@@ -7871,19 +7871,19 @@
         <v>5089.55788</v>
       </c>
       <c r="Q114">
-        <v>5321.098394290909</v>
+        <v>5323.552942100909</v>
       </c>
       <c r="R114">
         <v>6091.632138</v>
       </c>
       <c r="S114">
-        <v>5090.122174681818</v>
+        <v>5089.209807263636</v>
       </c>
       <c r="T114">
-        <v>11181.190018</v>
+        <v>-1002.074258</v>
       </c>
       <c r="U114">
-        <v>10411.22056897273</v>
+        <v>1281.070407564545</v>
       </c>
     </row>
     <row r="115" spans="1:21">
@@ -7936,19 +7936,19 @@
         <v>4889.18343</v>
       </c>
       <c r="Q115">
-        <v>5321.098394290909</v>
+        <v>5323.552942100909</v>
       </c>
       <c r="R115">
         <v>4650.975015</v>
       </c>
       <c r="S115">
-        <v>5090.122174681818</v>
+        <v>5089.209807263636</v>
       </c>
       <c r="T115">
-        <v>9540.158444999999</v>
+        <v>238.208415</v>
       </c>
       <c r="U115">
-        <v>10411.22056897273</v>
+        <v>1281.070407564545</v>
       </c>
     </row>
     <row r="116" spans="1:21">
@@ -8001,19 +8001,19 @@
         <v>3998.624197</v>
       </c>
       <c r="Q116">
-        <v>5321.098394290909</v>
+        <v>5323.552942100909</v>
       </c>
       <c r="R116">
         <v>4699.552101</v>
       </c>
       <c r="S116">
-        <v>5090.122174681818</v>
+        <v>5089.209807263636</v>
       </c>
       <c r="T116">
-        <v>8698.176298</v>
+        <v>-700.927904</v>
       </c>
       <c r="U116">
-        <v>10411.22056897273</v>
+        <v>1281.070407564545</v>
       </c>
     </row>
     <row r="117" spans="1:21">
@@ -8066,19 +8066,19 @@
         <v>4837.415762</v>
       </c>
       <c r="Q117">
-        <v>5321.098394290909</v>
+        <v>5323.552942100909</v>
       </c>
       <c r="R117">
         <v>4723.135796</v>
       </c>
       <c r="S117">
-        <v>5090.122174681818</v>
+        <v>5089.209807263636</v>
       </c>
       <c r="T117">
-        <v>9560.551557999999</v>
+        <v>114.279966</v>
       </c>
       <c r="U117">
-        <v>10411.22056897273</v>
+        <v>1281.070407564545</v>
       </c>
     </row>
     <row r="118" spans="1:21">
@@ -8131,19 +8131,19 @@
         <v>4668.00952733</v>
       </c>
       <c r="Q118">
-        <v>5321.098394290909</v>
+        <v>5323.552942100909</v>
       </c>
       <c r="R118">
         <v>6163.364678630001</v>
       </c>
       <c r="S118">
-        <v>5090.122174681818</v>
+        <v>5089.209807263636</v>
       </c>
       <c r="T118">
-        <v>10831.37420596</v>
+        <v>-1495.3551513</v>
       </c>
       <c r="U118">
-        <v>10411.22056897273</v>
+        <v>1281.070407564545</v>
       </c>
     </row>
     <row r="119" spans="1:21">
@@ -8196,19 +8196,19 @@
         <v>5349.607649340001</v>
       </c>
       <c r="Q119">
-        <v>5321.098394290909</v>
+        <v>5323.552942100909</v>
       </c>
       <c r="R119">
         <v>4363.012179560001</v>
       </c>
       <c r="S119">
-        <v>5090.122174681818</v>
+        <v>5089.209807263636</v>
       </c>
       <c r="T119">
-        <v>9712.6198289</v>
+        <v>986.5954697799999</v>
       </c>
       <c r="U119">
-        <v>10411.22056897273</v>
+        <v>1281.070407564545</v>
       </c>
     </row>
     <row r="120" spans="1:21">
@@ -8261,19 +8261,19 @@
         <v>5892.6712105</v>
       </c>
       <c r="Q120">
-        <v>5321.098394290909</v>
+        <v>5323.552942100909</v>
       </c>
       <c r="R120">
         <v>3408.68218244</v>
       </c>
       <c r="S120">
-        <v>5090.122174681818</v>
+        <v>5089.209807263636</v>
       </c>
       <c r="T120">
-        <v>9301.35339294</v>
+        <v>2483.98902806</v>
       </c>
       <c r="U120">
-        <v>10411.22056897273</v>
+        <v>1281.070407564545</v>
       </c>
     </row>
     <row r="121" spans="1:21">
@@ -8326,19 +8326,19 @@
         <v>4500.43265594</v>
       </c>
       <c r="Q121">
-        <v>5321.098394290909</v>
+        <v>5323.552942100909</v>
       </c>
       <c r="R121">
         <v>4114.75650827</v>
       </c>
       <c r="S121">
-        <v>5090.122174681818</v>
+        <v>5089.209807263636</v>
       </c>
       <c r="T121">
-        <v>8615.18916421</v>
+        <v>385.67614767</v>
       </c>
       <c r="U121">
-        <v>10411.22056897273</v>
+        <v>1281.070407564545</v>
       </c>
     </row>
     <row r="122" spans="1:21">
@@ -8388,22 +8388,22 @@
         <v>220.5339300775811</v>
       </c>
       <c r="P122">
-        <v>6163.99997409</v>
+        <v>6191</v>
       </c>
       <c r="Q122">
-        <v>5321.098394290909</v>
+        <v>5323.552942100909</v>
       </c>
       <c r="R122">
-        <v>5767.0360416</v>
+        <v>5757</v>
       </c>
       <c r="S122">
-        <v>5090.122174681818</v>
+        <v>5089.209807263636</v>
       </c>
       <c r="T122">
-        <v>11931.03601569</v>
+        <v>11948</v>
       </c>
       <c r="U122">
-        <v>10411.22056897273</v>
+        <v>1281.070407564545</v>
       </c>
     </row>
     <row r="123" spans="1:21">
@@ -8456,19 +8456,19 @@
         <v>6306.256318</v>
       </c>
       <c r="Q123">
-        <v>4898.377099109</v>
+        <v>5015.888271917273</v>
       </c>
       <c r="R123">
         <v>5987.389117</v>
       </c>
       <c r="S123">
-        <v>4645.848420576</v>
+        <v>4746.862200523637</v>
       </c>
       <c r="T123">
-        <v>12293.645435</v>
+        <v>318.867201</v>
       </c>
       <c r="U123">
-        <v>9544.225519685</v>
+        <v>1393.480616848182</v>
       </c>
     </row>
     <row r="124" spans="1:21">
@@ -8521,19 +8521,19 @@
         <v>6312.662723</v>
       </c>
       <c r="Q124">
-        <v>4898.377099109</v>
+        <v>5015.888271917273</v>
       </c>
       <c r="R124">
         <v>5436.515403</v>
       </c>
       <c r="S124">
-        <v>4645.848420576</v>
+        <v>4746.862200523637</v>
       </c>
       <c r="T124">
-        <v>11749.178126</v>
+        <v>876.14732</v>
       </c>
       <c r="U124">
-        <v>9544.225519685</v>
+        <v>1393.480616848182</v>
       </c>
     </row>
     <row r="125" spans="1:21">
@@ -8586,19 +8586,19 @@
         <v>4950.549545</v>
       </c>
       <c r="Q125">
-        <v>4898.377099109</v>
+        <v>5015.888271917273</v>
       </c>
       <c r="R125">
         <v>5411.689617</v>
       </c>
       <c r="S125">
-        <v>4645.848420576</v>
+        <v>4746.862200523637</v>
       </c>
       <c r="T125">
-        <v>10362.239162</v>
+        <v>-461.140072</v>
       </c>
       <c r="U125">
-        <v>9544.225519685</v>
+        <v>1393.480616848182</v>
       </c>
     </row>
     <row r="126" spans="1:21">
@@ -8651,19 +8651,19 @@
         <v>4502.277984</v>
       </c>
       <c r="Q126">
-        <v>4898.377099109</v>
+        <v>5015.888271917273</v>
       </c>
       <c r="R126">
         <v>4300.409404</v>
       </c>
       <c r="S126">
-        <v>4645.848420576</v>
+        <v>4746.862200523637</v>
       </c>
       <c r="T126">
-        <v>8802.687388</v>
+        <v>201.86858</v>
       </c>
       <c r="U126">
-        <v>9544.225519685</v>
+        <v>1393.480616848182</v>
       </c>
     </row>
     <row r="127" spans="1:21">
@@ -8716,19 +8716,19 @@
         <v>3429.332272</v>
       </c>
       <c r="Q127">
-        <v>4898.377099109</v>
+        <v>5015.888271917273</v>
       </c>
       <c r="R127">
         <v>4403.892992</v>
       </c>
       <c r="S127">
-        <v>4645.848420576</v>
+        <v>4746.862200523637</v>
       </c>
       <c r="T127">
-        <v>7833.225264</v>
+        <v>-974.5607199999999</v>
       </c>
       <c r="U127">
-        <v>9544.225519685</v>
+        <v>1393.480616848182</v>
       </c>
     </row>
     <row r="128" spans="1:21">
@@ -8781,19 +8781,19 @@
         <v>4649.443384</v>
       </c>
       <c r="Q128">
-        <v>4898.377099109</v>
+        <v>5015.888271917273</v>
       </c>
       <c r="R128">
         <v>4594.778166</v>
       </c>
       <c r="S128">
-        <v>4645.848420576</v>
+        <v>4746.862200523637</v>
       </c>
       <c r="T128">
-        <v>9244.22155</v>
+        <v>54.665218</v>
       </c>
       <c r="U128">
-        <v>9544.225519685</v>
+        <v>1393.480616848182</v>
       </c>
     </row>
     <row r="129" spans="1:21">
@@ -8846,19 +8846,19 @@
         <v>4578.420998699999</v>
       </c>
       <c r="Q129">
-        <v>4898.377099109</v>
+        <v>5015.888271917273</v>
       </c>
       <c r="R129">
         <v>5365.93059037</v>
       </c>
       <c r="S129">
-        <v>4645.848420576</v>
+        <v>4746.862200523637</v>
       </c>
       <c r="T129">
-        <v>9944.35158907</v>
+        <v>-787.50959167</v>
       </c>
       <c r="U129">
-        <v>9544.225519685</v>
+        <v>1393.480616848182</v>
       </c>
     </row>
     <row r="130" spans="1:21">
@@ -8911,19 +8911,19 @@
         <v>5336.41428693</v>
       </c>
       <c r="Q130">
-        <v>4898.377099109</v>
+        <v>5015.888271917273</v>
       </c>
       <c r="R130">
         <v>3916.87314604</v>
       </c>
       <c r="S130">
-        <v>4645.848420576</v>
+        <v>4746.862200523637</v>
       </c>
       <c r="T130">
-        <v>9253.287432969999</v>
+        <v>1419.54114089</v>
       </c>
       <c r="U130">
-        <v>9544.225519685</v>
+        <v>1393.480616848182</v>
       </c>
     </row>
     <row r="131" spans="1:21">
@@ -8976,19 +8976,19 @@
         <v>5374.34537988</v>
       </c>
       <c r="Q131">
-        <v>4898.377099109</v>
+        <v>5015.888271917273</v>
       </c>
       <c r="R131">
         <v>3133.06458335</v>
       </c>
       <c r="S131">
-        <v>4645.848420576</v>
+        <v>4746.862200523637</v>
       </c>
       <c r="T131">
-        <v>8507.40996323</v>
+        <v>2241.28079653</v>
       </c>
       <c r="U131">
-        <v>9544.225519685</v>
+        <v>1393.480616848182</v>
       </c>
     </row>
     <row r="132" spans="1:21">
@@ -9041,19 +9041,66 @@
         <v>3544.06809958</v>
       </c>
       <c r="Q132">
-        <v>4898.377099109</v>
+        <v>5015.888271917273</v>
       </c>
       <c r="R132">
         <v>3907.941187</v>
       </c>
       <c r="S132">
-        <v>4645.848420576</v>
+        <v>4746.862200523637</v>
       </c>
       <c r="T132">
-        <v>7452.00928658</v>
+        <v>-363.87308742</v>
       </c>
       <c r="U132">
-        <v>9544.225519685</v>
+        <v>1393.480616848182</v>
+      </c>
+    </row>
+    <row r="133" spans="1:21">
+      <c r="A133">
+        <v>12</v>
+      </c>
+      <c r="B133" t="s">
+        <v>32</v>
+      </c>
+      <c r="C133">
+        <v>2021</v>
+      </c>
+      <c r="J133">
+        <v>170.00381704316</v>
+      </c>
+      <c r="K133">
+        <v>165.47068406624</v>
+      </c>
+      <c r="L133">
+        <v>102.3848577974986</v>
+      </c>
+      <c r="M133">
+        <v>248.38308174534</v>
+      </c>
+      <c r="N133">
+        <v>123.94421688775</v>
+      </c>
+      <c r="O133">
+        <v>199.6054751216285</v>
+      </c>
+      <c r="P133">
+        <v>6191</v>
+      </c>
+      <c r="Q133">
+        <v>5015.888271917273</v>
+      </c>
+      <c r="R133">
+        <v>5757</v>
+      </c>
+      <c r="S133">
+        <v>4746.862200523637</v>
+      </c>
+      <c r="T133">
+        <v>12803</v>
+      </c>
+      <c r="U133">
+        <v>1393.480616848182</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
corrijo sobre-escritura del csv que repetia valores
</commit_message>
<xml_diff>
--- a/Estacionalidad/outputs/datossss.xlsx
+++ b/Estacionalidad/outputs/datossss.xlsx
@@ -8456,13 +8456,13 @@
         <v>6306.256318</v>
       </c>
       <c r="Q123">
-        <v>5015.888271917273</v>
+        <v>5051.888271917273</v>
       </c>
       <c r="R123">
         <v>5987.389117</v>
       </c>
       <c r="S123">
-        <v>4746.862200523637</v>
+        <v>4788.58947325091</v>
       </c>
       <c r="T123">
         <v>318.867201</v>
@@ -8521,13 +8521,13 @@
         <v>6312.662723</v>
       </c>
       <c r="Q124">
-        <v>5015.888271917273</v>
+        <v>5051.888271917273</v>
       </c>
       <c r="R124">
         <v>5436.515403</v>
       </c>
       <c r="S124">
-        <v>4746.862200523637</v>
+        <v>4788.58947325091</v>
       </c>
       <c r="T124">
         <v>876.14732</v>
@@ -8586,13 +8586,13 @@
         <v>4950.549545</v>
       </c>
       <c r="Q125">
-        <v>5015.888271917273</v>
+        <v>5051.888271917273</v>
       </c>
       <c r="R125">
         <v>5411.689617</v>
       </c>
       <c r="S125">
-        <v>4746.862200523637</v>
+        <v>4788.58947325091</v>
       </c>
       <c r="T125">
         <v>-461.140072</v>
@@ -8651,13 +8651,13 @@
         <v>4502.277984</v>
       </c>
       <c r="Q126">
-        <v>5015.888271917273</v>
+        <v>5051.888271917273</v>
       </c>
       <c r="R126">
         <v>4300.409404</v>
       </c>
       <c r="S126">
-        <v>4746.862200523637</v>
+        <v>4788.58947325091</v>
       </c>
       <c r="T126">
         <v>201.86858</v>
@@ -8716,13 +8716,13 @@
         <v>3429.332272</v>
       </c>
       <c r="Q127">
-        <v>5015.888271917273</v>
+        <v>5051.888271917273</v>
       </c>
       <c r="R127">
         <v>4403.892992</v>
       </c>
       <c r="S127">
-        <v>4746.862200523637</v>
+        <v>4788.58947325091</v>
       </c>
       <c r="T127">
         <v>-974.5607199999999</v>
@@ -8781,13 +8781,13 @@
         <v>4649.443384</v>
       </c>
       <c r="Q128">
-        <v>5015.888271917273</v>
+        <v>5051.888271917273</v>
       </c>
       <c r="R128">
         <v>4594.778166</v>
       </c>
       <c r="S128">
-        <v>4746.862200523637</v>
+        <v>4788.58947325091</v>
       </c>
       <c r="T128">
         <v>54.665218</v>
@@ -8846,13 +8846,13 @@
         <v>4578.420998699999</v>
       </c>
       <c r="Q129">
-        <v>5015.888271917273</v>
+        <v>5051.888271917273</v>
       </c>
       <c r="R129">
         <v>5365.93059037</v>
       </c>
       <c r="S129">
-        <v>4746.862200523637</v>
+        <v>4788.58947325091</v>
       </c>
       <c r="T129">
         <v>-787.50959167</v>
@@ -8911,13 +8911,13 @@
         <v>5336.41428693</v>
       </c>
       <c r="Q130">
-        <v>5015.888271917273</v>
+        <v>5051.888271917273</v>
       </c>
       <c r="R130">
         <v>3916.87314604</v>
       </c>
       <c r="S130">
-        <v>4746.862200523637</v>
+        <v>4788.58947325091</v>
       </c>
       <c r="T130">
         <v>1419.54114089</v>
@@ -8976,13 +8976,13 @@
         <v>5374.34537988</v>
       </c>
       <c r="Q131">
-        <v>5015.888271917273</v>
+        <v>5051.888271917273</v>
       </c>
       <c r="R131">
         <v>3133.06458335</v>
       </c>
       <c r="S131">
-        <v>4746.862200523637</v>
+        <v>4788.58947325091</v>
       </c>
       <c r="T131">
         <v>2241.28079653</v>
@@ -9041,13 +9041,13 @@
         <v>3544.06809958</v>
       </c>
       <c r="Q132">
-        <v>5015.888271917273</v>
+        <v>5051.888271917273</v>
       </c>
       <c r="R132">
         <v>3907.941187</v>
       </c>
       <c r="S132">
-        <v>4746.862200523637</v>
+        <v>4788.58947325091</v>
       </c>
       <c r="T132">
         <v>-363.87308742</v>
@@ -9085,16 +9085,16 @@
         <v>199.6054751216285</v>
       </c>
       <c r="P133">
-        <v>6191</v>
+        <v>6587</v>
       </c>
       <c r="Q133">
-        <v>5015.888271917273</v>
+        <v>5051.888271917273</v>
       </c>
       <c r="R133">
-        <v>5757</v>
+        <v>6216</v>
       </c>
       <c r="S133">
-        <v>4746.862200523637</v>
+        <v>4788.58947325091</v>
       </c>
       <c r="T133">
         <v>12803</v>

</xml_diff>

<commit_message>
Se actualiza la serie de intercambio comercial, M nov 2021.
</commit_message>
<xml_diff>
--- a/Estacionalidad/outputs/datossss.xlsx
+++ b/Estacionalidad/outputs/datossss.xlsx
@@ -10249,19 +10249,19 @@
         <v>6493.159464</v>
       </c>
       <c r="W112">
-        <v>5323.552942100909</v>
+        <v>5323.570049492728</v>
       </c>
       <c r="X112">
         <v>6229.740888</v>
       </c>
       <c r="Y112">
-        <v>5089.209807263636</v>
+        <v>5090.122174681818</v>
       </c>
       <c r="Z112">
         <v>263.418576</v>
       </c>
       <c r="AA112">
-        <v>1281.070407564545</v>
+        <v>233.4478748109091</v>
       </c>
       <c r="AB112">
         <v>0.09768459928049822</v>
@@ -10338,19 +10338,19 @@
         <v>6649.420587</v>
       </c>
       <c r="W113">
-        <v>5323.552942100909</v>
+        <v>5323.570049492728</v>
       </c>
       <c r="X113">
         <v>5779.456393</v>
       </c>
       <c r="Y113">
-        <v>5089.209807263636</v>
+        <v>5090.122174681818</v>
       </c>
       <c r="Z113">
         <v>869.964194</v>
       </c>
       <c r="AA113">
-        <v>1281.070407564545</v>
+        <v>233.4478748109091</v>
       </c>
       <c r="AB113">
         <v>0.02406549906349253</v>
@@ -10427,19 +10427,19 @@
         <v>5089.55788</v>
       </c>
       <c r="W114">
-        <v>5323.552942100909</v>
+        <v>5323.570049492728</v>
       </c>
       <c r="X114">
         <v>6091.632138</v>
       </c>
       <c r="Y114">
-        <v>5089.209807263636</v>
+        <v>5090.122174681818</v>
       </c>
       <c r="Z114">
         <v>-1002.074258</v>
       </c>
       <c r="AA114">
-        <v>1281.070407564545</v>
+        <v>233.4478748109091</v>
       </c>
       <c r="AB114">
         <v>-0.2345862600494276</v>
@@ -10516,19 +10516,19 @@
         <v>4889.18343</v>
       </c>
       <c r="W115">
-        <v>5323.552942100909</v>
+        <v>5323.570049492728</v>
       </c>
       <c r="X115">
         <v>4650.975015</v>
       </c>
       <c r="Y115">
-        <v>5089.209807263636</v>
+        <v>5090.122174681818</v>
       </c>
       <c r="Z115">
         <v>238.208415</v>
       </c>
       <c r="AA115">
-        <v>1281.070407564545</v>
+        <v>233.4478748109091</v>
       </c>
       <c r="AB115">
         <v>-0.03936971633378894</v>
@@ -10605,19 +10605,19 @@
         <v>3998.624197</v>
       </c>
       <c r="W116">
-        <v>5323.552942100909</v>
+        <v>5323.570049492728</v>
       </c>
       <c r="X116">
         <v>4699.552101</v>
       </c>
       <c r="Y116">
-        <v>5089.209807263636</v>
+        <v>5090.122174681818</v>
       </c>
       <c r="Z116">
         <v>-700.927904</v>
       </c>
       <c r="AA116">
-        <v>1281.070407564545</v>
+        <v>233.4478748109091</v>
       </c>
       <c r="AB116">
         <v>-0.1821488691824352</v>
@@ -10694,19 +10694,19 @@
         <v>4837.415762</v>
       </c>
       <c r="W117">
-        <v>5323.552942100909</v>
+        <v>5323.570049492728</v>
       </c>
       <c r="X117">
         <v>4723.135796</v>
       </c>
       <c r="Y117">
-        <v>5089.209807263636</v>
+        <v>5090.122174681818</v>
       </c>
       <c r="Z117">
         <v>114.279966</v>
       </c>
       <c r="AA117">
-        <v>1281.070407564545</v>
+        <v>233.4478748109091</v>
       </c>
       <c r="AB117">
         <v>0.2097700418132091</v>
@@ -10783,19 +10783,19 @@
         <v>4668.00952733</v>
       </c>
       <c r="W118">
-        <v>5323.552942100909</v>
+        <v>5323.570049492728</v>
       </c>
       <c r="X118">
         <v>6163.364678630001</v>
       </c>
       <c r="Y118">
-        <v>5089.209807263636</v>
+        <v>5090.122174681818</v>
       </c>
       <c r="Z118">
         <v>-1495.3551513</v>
       </c>
       <c r="AA118">
-        <v>1281.070407564545</v>
+        <v>233.4478748109091</v>
       </c>
       <c r="AB118">
         <v>-0.0350199864979065</v>
@@ -10872,19 +10872,19 @@
         <v>5349.607649340001</v>
       </c>
       <c r="W119">
-        <v>5323.552942100909</v>
+        <v>5323.570049492728</v>
       </c>
       <c r="X119">
         <v>4363.012179560001</v>
       </c>
       <c r="Y119">
-        <v>5089.209807263636</v>
+        <v>5090.122174681818</v>
       </c>
       <c r="Z119">
         <v>986.5954697799999</v>
       </c>
       <c r="AA119">
-        <v>1281.070407564545</v>
+        <v>233.4478748109091</v>
       </c>
       <c r="AB119">
         <v>0.146014723838805</v>
@@ -10961,19 +10961,19 @@
         <v>5892.6712105</v>
       </c>
       <c r="W120">
-        <v>5323.552942100909</v>
+        <v>5323.570049492728</v>
       </c>
       <c r="X120">
         <v>3408.68218244</v>
       </c>
       <c r="Y120">
-        <v>5089.209807263636</v>
+        <v>5090.122174681818</v>
       </c>
       <c r="Z120">
         <v>2483.98902806</v>
       </c>
       <c r="AA120">
-        <v>1281.070407564545</v>
+        <v>233.4478748109091</v>
       </c>
       <c r="AB120">
         <v>0.1015146524300712</v>
@@ -11050,19 +11050,19 @@
         <v>4500.43265594</v>
       </c>
       <c r="W121">
-        <v>5323.552942100909</v>
+        <v>5323.570049492728</v>
       </c>
       <c r="X121">
         <v>4114.75650827</v>
       </c>
       <c r="Y121">
-        <v>5089.209807263636</v>
+        <v>5090.122174681818</v>
       </c>
       <c r="Z121">
         <v>385.67614767</v>
       </c>
       <c r="AA121">
-        <v>1281.070407564545</v>
+        <v>233.4478748109091</v>
       </c>
       <c r="AB121">
         <v>-0.2362661185099223</v>
@@ -11136,28 +11136,28 @@
         <v>220.5339300775811</v>
       </c>
       <c r="V122">
-        <v>6191</v>
+        <v>6191.188181310001</v>
       </c>
       <c r="W122">
-        <v>5323.552942100909</v>
+        <v>5323.570049492728</v>
       </c>
       <c r="X122">
-        <v>5757</v>
+        <v>5767.0360416</v>
       </c>
       <c r="Y122">
-        <v>5089.209807263636</v>
+        <v>5090.122174681818</v>
       </c>
       <c r="Z122">
-        <v>11948</v>
+        <v>424.15213971</v>
       </c>
       <c r="AA122">
-        <v>1281.070407564545</v>
+        <v>233.4478748109091</v>
       </c>
       <c r="AB122">
-        <v>0.375645515288106</v>
+        <v>0.3756873293367513</v>
       </c>
       <c r="AC122">
-        <v>0.3991107343604303</v>
+        <v>0.4015497709303537</v>
       </c>
     </row>
     <row r="123" spans="1:29">
@@ -11210,19 +11210,19 @@
         <v>6306.256318</v>
       </c>
       <c r="W123">
-        <v>5051.888271917273</v>
+        <v>5051.888272472727</v>
       </c>
       <c r="X123">
         <v>5987.389117</v>
       </c>
       <c r="Y123">
-        <v>4788.58947325091</v>
+        <v>4788.565382631818</v>
       </c>
       <c r="Z123">
         <v>318.867201</v>
       </c>
       <c r="AA123">
-        <v>1393.480616848182</v>
+        <v>263.3228898409092</v>
       </c>
       <c r="AB123">
         <v>0.1499318116784303</v>
@@ -11299,19 +11299,19 @@
         <v>6312.662723</v>
       </c>
       <c r="W124">
-        <v>5051.888271917273</v>
+        <v>5051.888272472727</v>
       </c>
       <c r="X124">
         <v>5436.515403</v>
       </c>
       <c r="Y124">
-        <v>4788.58947325091</v>
+        <v>4788.565382631818</v>
       </c>
       <c r="Z124">
         <v>876.14732</v>
       </c>
       <c r="AA124">
-        <v>1393.480616848182</v>
+        <v>263.3228898409092</v>
       </c>
       <c r="AB124">
         <v>0.001015880845457229</v>
@@ -11388,19 +11388,19 @@
         <v>4950.549545</v>
       </c>
       <c r="W125">
-        <v>5051.888271917273</v>
+        <v>5051.888272472727</v>
       </c>
       <c r="X125">
         <v>5411.689617</v>
       </c>
       <c r="Y125">
-        <v>4788.58947325091</v>
+        <v>4788.565382631818</v>
       </c>
       <c r="Z125">
         <v>-461.140072</v>
       </c>
       <c r="AA125">
-        <v>1393.480616848182</v>
+        <v>263.3228898409092</v>
       </c>
       <c r="AB125">
         <v>-0.2157747432057761</v>
@@ -11477,19 +11477,19 @@
         <v>4502.277984</v>
       </c>
       <c r="W126">
-        <v>5051.888271917273</v>
+        <v>5051.888272472727</v>
       </c>
       <c r="X126">
         <v>4300.409404</v>
       </c>
       <c r="Y126">
-        <v>4788.58947325091</v>
+        <v>4788.565382631818</v>
       </c>
       <c r="Z126">
         <v>201.86858</v>
       </c>
       <c r="AA126">
-        <v>1393.480616848182</v>
+        <v>263.3228898409092</v>
       </c>
       <c r="AB126">
         <v>-0.09054985854100772</v>
@@ -11566,19 +11566,19 @@
         <v>3429.332272</v>
       </c>
       <c r="W127">
-        <v>5051.888271917273</v>
+        <v>5051.888272472727</v>
       </c>
       <c r="X127">
         <v>4403.892992</v>
       </c>
       <c r="Y127">
-        <v>4788.58947325091</v>
+        <v>4788.565382631818</v>
       </c>
       <c r="Z127">
         <v>-974.5607199999999</v>
       </c>
       <c r="AA127">
-        <v>1393.480616848182</v>
+        <v>263.3228898409092</v>
       </c>
       <c r="AB127">
         <v>-0.2383117425918586</v>
@@ -11655,19 +11655,19 @@
         <v>4649.443384</v>
       </c>
       <c r="W128">
-        <v>5051.888271917273</v>
+        <v>5051.888272472727</v>
       </c>
       <c r="X128">
         <v>4594.778166</v>
       </c>
       <c r="Y128">
-        <v>4788.58947325091</v>
+        <v>4788.565382631818</v>
       </c>
       <c r="Z128">
         <v>54.665218</v>
       </c>
       <c r="AA128">
-        <v>1393.480616848182</v>
+        <v>263.3228898409092</v>
       </c>
       <c r="AB128">
         <v>0.3557867874052421</v>
@@ -11744,19 +11744,19 @@
         <v>4578.420998699999</v>
       </c>
       <c r="W129">
-        <v>5051.888271917273</v>
+        <v>5051.888272472727</v>
       </c>
       <c r="X129">
         <v>5365.93059037</v>
       </c>
       <c r="Y129">
-        <v>4788.58947325091</v>
+        <v>4788.565382631818</v>
       </c>
       <c r="Z129">
         <v>-787.50959167</v>
       </c>
       <c r="AA129">
-        <v>1393.480616848182</v>
+        <v>263.3228898409092</v>
       </c>
       <c r="AB129">
         <v>-0.0152754597559801</v>
@@ -11833,19 +11833,19 @@
         <v>5336.41428693</v>
       </c>
       <c r="W130">
-        <v>5051.888271917273</v>
+        <v>5051.888272472727</v>
       </c>
       <c r="X130">
         <v>3916.87314604</v>
       </c>
       <c r="Y130">
-        <v>4788.58947325091</v>
+        <v>4788.565382631818</v>
       </c>
       <c r="Z130">
         <v>1419.54114089</v>
       </c>
       <c r="AA130">
-        <v>1393.480616848182</v>
+        <v>263.3228898409092</v>
       </c>
       <c r="AB130">
         <v>0.1655577956778604</v>
@@ -11922,19 +11922,19 @@
         <v>5374.34537988</v>
       </c>
       <c r="W131">
-        <v>5051.888271917273</v>
+        <v>5051.888272472727</v>
       </c>
       <c r="X131">
         <v>3133.06458335</v>
       </c>
       <c r="Y131">
-        <v>4788.58947325091</v>
+        <v>4788.565382631818</v>
       </c>
       <c r="Z131">
         <v>2241.28079653</v>
       </c>
       <c r="AA131">
-        <v>1393.480616848182</v>
+        <v>263.3228898409092</v>
       </c>
       <c r="AB131">
         <v>0.007107973802352729</v>
@@ -12011,19 +12011,19 @@
         <v>3544.06809958</v>
       </c>
       <c r="W132">
-        <v>5051.888271917273</v>
+        <v>5051.888272472727</v>
       </c>
       <c r="X132">
         <v>3907.941187</v>
       </c>
       <c r="Y132">
-        <v>4788.58947325091</v>
+        <v>4788.565382631818</v>
       </c>
       <c r="Z132">
         <v>-363.87308742</v>
       </c>
       <c r="AA132">
-        <v>1393.480616848182</v>
+        <v>263.3228898409092</v>
       </c>
       <c r="AB132">
         <v>-0.3405581798207519</v>
@@ -12061,28 +12061,28 @@
         <v>199.6054751216285</v>
       </c>
       <c r="V133">
-        <v>6587</v>
+        <v>6587.00000611</v>
       </c>
       <c r="W133">
-        <v>5051.888271917273</v>
+        <v>5051.888272472727</v>
       </c>
       <c r="X133">
-        <v>6216</v>
+        <v>6215.73500319</v>
       </c>
       <c r="Y133">
-        <v>4788.58947325091</v>
+        <v>4788.565382631818</v>
       </c>
       <c r="Z133">
-        <v>12803</v>
+        <v>371.26500292</v>
       </c>
       <c r="AA133">
-        <v>1393.480616848182</v>
+        <v>263.3228898409092</v>
       </c>
       <c r="AB133">
-        <v>0.8585985976907757</v>
+        <v>0.8585985994147831</v>
       </c>
       <c r="AC133">
-        <v>0.5906073562923351</v>
+        <v>0.5905395464668235</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
agrego variaciones, se rompe por inconsistencia de nombres en df
</commit_message>
<xml_diff>
--- a/Estacionalidad/outputs/datossss.xlsx
+++ b/Estacionalidad/outputs/datossss.xlsx
@@ -28,19 +28,19 @@
     <t>iv_x</t>
   </si>
   <si>
-    <t>p_expo</t>
+    <t>ip_x</t>
   </si>
   <si>
-    <t>q_expo</t>
+    <t>iq_x</t>
   </si>
   <si>
     <t>iv_m</t>
   </si>
   <si>
-    <t>p_impo</t>
+    <t>ip_m</t>
   </si>
   <si>
-    <t>q_impo</t>
+    <t>iq_m</t>
   </si>
   <si>
     <t>iv_x_var</t>
@@ -61,22 +61,22 @@
     <t>iq_m_var</t>
   </si>
   <si>
-    <t>iv_expo_media</t>
+    <t>iv_x_media</t>
   </si>
   <si>
-    <t>p_expo_media</t>
+    <t>ip_x_media</t>
   </si>
   <si>
-    <t>q_expo_media</t>
+    <t>iq_x_media</t>
   </si>
   <si>
-    <t>iv_impo_media</t>
+    <t>iv_m_media</t>
   </si>
   <si>
-    <t>p_impo_media</t>
+    <t>p_m_media</t>
   </si>
   <si>
-    <t>q_impo_media</t>
+    <t>q_m_media</t>
   </si>
   <si>
     <t>v_expo</t>
@@ -97,10 +97,10 @@
     <t>v_ic_media</t>
   </si>
   <si>
-    <t>vX_var</t>
+    <t>v_expo_var</t>
   </si>
   <si>
-    <t>vM_var</t>
+    <t>v_impo_var</t>
   </si>
   <si>
     <t>ene</t>

</xml_diff>

<commit_message>
Variacion queda completamente funcional
</commit_message>
<xml_diff>
--- a/Estacionalidad/outputs/datossss.xlsx
+++ b/Estacionalidad/outputs/datossss.xlsx
@@ -73,10 +73,10 @@
     <t>iv_m_media</t>
   </si>
   <si>
-    <t>p_m_media</t>
+    <t>ip_m_media</t>
   </si>
   <si>
-    <t>q_m_media</t>
+    <t>iq_m_media</t>
   </si>
   <si>
     <t>v_expo</t>

</xml_diff>

<commit_message>
pyq expo, pyq impo e iti
</commit_message>
<xml_diff>
--- a/Estacionalidad/outputs/datossss.xlsx
+++ b/Estacionalidad/outputs/datossss.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="44">
   <si>
     <t>Mes_num</t>
   </si>
@@ -101,6 +101,15 @@
   </si>
   <si>
     <t>v_impo_var</t>
+  </si>
+  <si>
+    <t>ITI</t>
+  </si>
+  <si>
+    <t>ITI_var</t>
+  </si>
+  <si>
+    <t>ITI_media</t>
   </si>
   <si>
     <t>ene</t>
@@ -494,13 +503,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AC133"/>
+  <dimension ref="A1:AF133"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:29">
+    <row r="1" spans="1:32">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -588,13 +597,22 @@
       <c r="AC1" s="1" t="s">
         <v>28</v>
       </c>
+      <c r="AD1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>31</v>
+      </c>
     </row>
-    <row r="2" spans="1:29">
+    <row r="2" spans="1:32">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C2">
         <v>2011</v>
@@ -659,13 +677,22 @@
       <c r="AC2">
         <v>0.523502361382775</v>
       </c>
+      <c r="AD2">
+        <v>140.1470898191464</v>
+      </c>
+      <c r="AE2">
+        <v>0.03748339012382873</v>
+      </c>
+      <c r="AF2">
+        <v>137.6455277471591</v>
+      </c>
     </row>
-    <row r="3" spans="1:29">
+    <row r="3" spans="1:32">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C3">
         <v>2012</v>
@@ -748,13 +775,22 @@
       <c r="AC3">
         <v>0.0970600947957887</v>
       </c>
+      <c r="AD3">
+        <v>145.295026524668</v>
+      </c>
+      <c r="AE3">
+        <v>0.03673238389869393</v>
+      </c>
+      <c r="AF3">
+        <v>137.6455277471591</v>
+      </c>
     </row>
-    <row r="4" spans="1:29">
+    <row r="4" spans="1:32">
       <c r="A4">
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C4">
         <v>2013</v>
@@ -837,13 +873,22 @@
       <c r="AC4">
         <v>-0.001030129211186281</v>
       </c>
+      <c r="AD4">
+        <v>145.0802108603752</v>
+      </c>
+      <c r="AE4">
+        <v>-0.00147847912919663</v>
+      </c>
+      <c r="AF4">
+        <v>137.6455277471591</v>
+      </c>
     </row>
-    <row r="5" spans="1:29">
+    <row r="5" spans="1:32">
       <c r="A5">
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C5">
         <v>2014</v>
@@ -926,13 +971,22 @@
       <c r="AC5">
         <v>0.05419765291243084</v>
       </c>
+      <c r="AD5">
+        <v>136.0155548247364</v>
+      </c>
+      <c r="AE5">
+        <v>-0.06248030645862945</v>
+      </c>
+      <c r="AF5">
+        <v>137.6455277471591</v>
+      </c>
     </row>
-    <row r="6" spans="1:29">
+    <row r="6" spans="1:32">
       <c r="A6">
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C6">
         <v>2015</v>
@@ -1015,13 +1069,22 @@
       <c r="AC6">
         <v>-0.2276527347088668</v>
       </c>
+      <c r="AD6">
+        <v>134.8203494953468</v>
+      </c>
+      <c r="AE6">
+        <v>-0.008787269448186974</v>
+      </c>
+      <c r="AF6">
+        <v>137.6455277471591</v>
+      </c>
     </row>
-    <row r="7" spans="1:29">
+    <row r="7" spans="1:32">
       <c r="A7">
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C7">
         <v>2016</v>
@@ -1104,13 +1167,22 @@
       <c r="AC7">
         <v>-0.05488181263505887</v>
       </c>
+      <c r="AD7">
+        <v>126.4312873255282</v>
+      </c>
+      <c r="AE7">
+        <v>-0.06222400550970297</v>
+      </c>
+      <c r="AF7">
+        <v>137.6455277471591</v>
+      </c>
     </row>
-    <row r="8" spans="1:29">
+    <row r="8" spans="1:32">
       <c r="A8">
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C8">
         <v>2017</v>
@@ -1193,13 +1265,22 @@
       <c r="AC8">
         <v>0.0535637454354394</v>
       </c>
+      <c r="AD8">
+        <v>134.0277117985371</v>
+      </c>
+      <c r="AE8">
+        <v>0.06008342265352407</v>
+      </c>
+      <c r="AF8">
+        <v>137.6455277471591</v>
+      </c>
     </row>
-    <row r="9" spans="1:29">
+    <row r="9" spans="1:32">
       <c r="A9">
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C9">
         <v>2018</v>
@@ -1282,13 +1363,22 @@
       <c r="AC9">
         <v>0.3220787527470592</v>
       </c>
+      <c r="AD9">
+        <v>136.4047285091626</v>
+      </c>
+      <c r="AE9">
+        <v>0.01773526294471495</v>
+      </c>
+      <c r="AF9">
+        <v>137.6455277471591</v>
+      </c>
     </row>
-    <row r="10" spans="1:29">
+    <row r="10" spans="1:32">
       <c r="A10">
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C10">
         <v>2019</v>
@@ -1371,13 +1461,22 @@
       <c r="AC10">
         <v>-0.2666527493323592</v>
       </c>
+      <c r="AD10">
+        <v>130.3537178049512</v>
+      </c>
+      <c r="AE10">
+        <v>-0.04436071073448844</v>
+      </c>
+      <c r="AF10">
+        <v>137.6455277471591</v>
+      </c>
     </row>
-    <row r="11" spans="1:29">
+    <row r="11" spans="1:32">
       <c r="A11">
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C11">
         <v>2020</v>
@@ -1460,13 +1559,22 @@
       <c r="AC11">
         <v>-0.1605897398396399</v>
       </c>
+      <c r="AD11">
+        <v>136.6772149141131</v>
+      </c>
+      <c r="AE11">
+        <v>0.04851029349714264</v>
+      </c>
+      <c r="AF11">
+        <v>137.6455277471591</v>
+      </c>
     </row>
-    <row r="12" spans="1:29">
+    <row r="12" spans="1:32">
       <c r="A12">
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C12">
         <v>2021</v>
@@ -1549,13 +1657,22 @@
       <c r="AC12">
         <v>0.08715013619534617</v>
       </c>
+      <c r="AD12">
+        <v>148.8479133421853</v>
+      </c>
+      <c r="AE12">
+        <v>0.08904701808359339</v>
+      </c>
+      <c r="AF12">
+        <v>137.6455277471591</v>
+      </c>
     </row>
-    <row r="13" spans="1:29">
+    <row r="13" spans="1:32">
       <c r="A13">
         <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C13">
         <v>2011</v>
@@ -1620,13 +1737,22 @@
       <c r="AC13">
         <v>0.3789288947409792</v>
       </c>
+      <c r="AD13">
+        <v>140.3663001604104</v>
+      </c>
+      <c r="AE13">
+        <v>0.0927934113387987</v>
+      </c>
+      <c r="AF13">
+        <v>134.9208881376577</v>
+      </c>
     </row>
-    <row r="14" spans="1:29">
+    <row r="14" spans="1:32">
       <c r="A14">
         <v>2</v>
       </c>
       <c r="B14" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C14">
         <v>2012</v>
@@ -1709,13 +1835,22 @@
       <c r="AC14">
         <v>-0.008250503955039457</v>
       </c>
+      <c r="AD14">
+        <v>143.264458918516</v>
+      </c>
+      <c r="AE14">
+        <v>0.02064711226835469</v>
+      </c>
+      <c r="AF14">
+        <v>134.9208881376577</v>
+      </c>
     </row>
-    <row r="15" spans="1:29">
+    <row r="15" spans="1:32">
       <c r="A15">
         <v>2</v>
       </c>
       <c r="B15" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C15">
         <v>2013</v>
@@ -1798,13 +1933,22 @@
       <c r="AC15">
         <v>0.09518888554801919</v>
       </c>
+      <c r="AD15">
+        <v>139.3355720035588</v>
+      </c>
+      <c r="AE15">
+        <v>-0.02742401670739392</v>
+      </c>
+      <c r="AF15">
+        <v>134.9208881376577</v>
+      </c>
     </row>
-    <row r="16" spans="1:29">
+    <row r="16" spans="1:32">
       <c r="A16">
         <v>2</v>
       </c>
       <c r="B16" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C16">
         <v>2014</v>
@@ -1887,13 +2031,22 @@
       <c r="AC16">
         <v>0.07009174026786802</v>
       </c>
+      <c r="AD16">
+        <v>138.9203344590518</v>
+      </c>
+      <c r="AE16">
+        <v>-0.002980125882688589</v>
+      </c>
+      <c r="AF16">
+        <v>134.9208881376577</v>
+      </c>
     </row>
-    <row r="17" spans="1:29">
+    <row r="17" spans="1:32">
       <c r="A17">
         <v>2</v>
       </c>
       <c r="B17" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C17">
         <v>2015</v>
@@ -1976,13 +2129,22 @@
       <c r="AC17">
         <v>-0.262387042966275</v>
       </c>
+      <c r="AD17">
+        <v>128.1568853055665</v>
+      </c>
+      <c r="AE17">
+        <v>-0.07747929196541037</v>
+      </c>
+      <c r="AF17">
+        <v>134.9208881376577</v>
+      </c>
     </row>
-    <row r="18" spans="1:29">
+    <row r="18" spans="1:32">
       <c r="A18">
         <v>2</v>
       </c>
       <c r="B18" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C18">
         <v>2016</v>
@@ -2065,13 +2227,22 @@
       <c r="AC18">
         <v>0.00286165453031173</v>
       </c>
+      <c r="AD18">
+        <v>129.5314861018409</v>
+      </c>
+      <c r="AE18">
+        <v>0.01072592231776648</v>
+      </c>
+      <c r="AF18">
+        <v>134.9208881376577</v>
+      </c>
     </row>
-    <row r="19" spans="1:29">
+    <row r="19" spans="1:32">
       <c r="A19">
         <v>2</v>
       </c>
       <c r="B19" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C19">
         <v>2017</v>
@@ -2154,13 +2325,22 @@
       <c r="AC19">
         <v>0.005124722916995283</v>
       </c>
+      <c r="AD19">
+        <v>128.0978268857293</v>
+      </c>
+      <c r="AE19">
+        <v>-0.01106803650028665</v>
+      </c>
+      <c r="AF19">
+        <v>134.9208881376577</v>
+      </c>
     </row>
-    <row r="20" spans="1:29">
+    <row r="20" spans="1:32">
       <c r="A20">
         <v>2</v>
       </c>
       <c r="B20" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C20">
         <v>2018</v>
@@ -2243,13 +2423,22 @@
       <c r="AC20">
         <v>0.262027535498794</v>
       </c>
+      <c r="AD20">
+        <v>129.1442967864538</v>
+      </c>
+      <c r="AE20">
+        <v>0.008169302525779631</v>
+      </c>
+      <c r="AF20">
+        <v>134.9208881376577</v>
+      </c>
     </row>
-    <row r="21" spans="1:29">
+    <row r="21" spans="1:32">
       <c r="A21">
         <v>2</v>
       </c>
       <c r="B21" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C21">
         <v>2019</v>
@@ -2332,13 +2521,22 @@
       <c r="AC21">
         <v>-0.2305710800642351</v>
       </c>
+      <c r="AD21">
+        <v>128.1122625108115</v>
+      </c>
+      <c r="AE21">
+        <v>-0.007991326766437434</v>
+      </c>
+      <c r="AF21">
+        <v>134.9208881376577</v>
+      </c>
     </row>
-    <row r="22" spans="1:29">
+    <row r="22" spans="1:32">
       <c r="A22">
         <v>2</v>
       </c>
       <c r="B22" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C22">
         <v>2020</v>
@@ -2421,13 +2619,22 @@
       <c r="AC22">
         <v>-0.2017823513879426</v>
       </c>
+      <c r="AD22">
+        <v>129.4934881700457</v>
+      </c>
+      <c r="AE22">
+        <v>0.01078136965317933</v>
+      </c>
+      <c r="AF22">
+        <v>134.9208881376577</v>
+      </c>
     </row>
-    <row r="23" spans="1:29">
+    <row r="23" spans="1:32">
       <c r="A23">
         <v>2</v>
       </c>
       <c r="B23" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C23">
         <v>2021</v>
@@ -2510,13 +2717,22 @@
       <c r="AC23">
         <v>0.1634019828879179</v>
       </c>
+      <c r="AD23">
+        <v>149.70685821225</v>
+      </c>
+      <c r="AE23">
+        <v>0.1560956487299259</v>
+      </c>
+      <c r="AF23">
+        <v>134.9208881376577</v>
+      </c>
     </row>
-    <row r="24" spans="1:29">
+    <row r="24" spans="1:32">
       <c r="A24">
         <v>3</v>
       </c>
       <c r="B24" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C24">
         <v>2011</v>
@@ -2581,13 +2797,22 @@
       <c r="AC24">
         <v>0.2813500789795134</v>
       </c>
+      <c r="AD24">
+        <v>139.9492081059655</v>
+      </c>
+      <c r="AE24">
+        <v>0.1274221133773965</v>
+      </c>
+      <c r="AF24">
+        <v>134.0265105079613</v>
+      </c>
     </row>
-    <row r="25" spans="1:29">
+    <row r="25" spans="1:32">
       <c r="A25">
         <v>3</v>
       </c>
       <c r="B25" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C25">
         <v>2012</v>
@@ -2670,13 +2895,22 @@
       <c r="AC25">
         <v>-0.08775581007767985</v>
       </c>
+      <c r="AD25">
+        <v>148.2614535552861</v>
+      </c>
+      <c r="AE25">
+        <v>0.05939473014400232</v>
+      </c>
+      <c r="AF25">
+        <v>134.0265105079613</v>
+      </c>
     </row>
-    <row r="26" spans="1:29">
+    <row r="26" spans="1:32">
       <c r="A26">
         <v>3</v>
       </c>
       <c r="B26" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C26">
         <v>2013</v>
@@ -2759,13 +2993,22 @@
       <c r="AC26">
         <v>0.09184292861445686</v>
       </c>
+      <c r="AD26">
+        <v>138.8518678185956</v>
+      </c>
+      <c r="AE26">
+        <v>-0.06346616407063399</v>
+      </c>
+      <c r="AF26">
+        <v>134.0265105079613</v>
+      </c>
     </row>
-    <row r="27" spans="1:29">
+    <row r="27" spans="1:32">
       <c r="A27">
         <v>3</v>
       </c>
       <c r="B27" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C27">
         <v>2014</v>
@@ -2848,13 +3091,22 @@
       <c r="AC27">
         <v>-0.04080451055973067</v>
       </c>
+      <c r="AD27">
+        <v>128.5254227924407</v>
+      </c>
+      <c r="AE27">
+        <v>-0.07437022769939294</v>
+      </c>
+      <c r="AF27">
+        <v>134.0265105079613</v>
+      </c>
     </row>
-    <row r="28" spans="1:29">
+    <row r="28" spans="1:32">
       <c r="A28">
         <v>3</v>
       </c>
       <c r="B28" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C28">
         <v>2015</v>
@@ -2937,13 +3189,22 @@
       <c r="AC28">
         <v>-0.0614245228662319</v>
       </c>
+      <c r="AD28">
+        <v>124.7575712005926</v>
+      </c>
+      <c r="AE28">
+        <v>-0.02931600231288767</v>
+      </c>
+      <c r="AF28">
+        <v>134.0265105079613</v>
+      </c>
     </row>
-    <row r="29" spans="1:29">
+    <row r="29" spans="1:32">
       <c r="A29">
         <v>3</v>
       </c>
       <c r="B29" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C29">
         <v>2016</v>
@@ -3026,13 +3287,22 @@
       <c r="AC29">
         <v>-0.09932887940633817</v>
       </c>
+      <c r="AD29">
+        <v>130.0414384088916</v>
+      </c>
+      <c r="AE29">
+        <v>0.04235307851419523</v>
+      </c>
+      <c r="AF29">
+        <v>134.0265105079613</v>
+      </c>
     </row>
-    <row r="30" spans="1:29">
+    <row r="30" spans="1:32">
       <c r="A30">
         <v>3</v>
       </c>
       <c r="B30" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C30">
         <v>2017</v>
@@ -3115,13 +3385,22 @@
       <c r="AC30">
         <v>0.2016234471396983</v>
       </c>
+      <c r="AD30">
+        <v>129.731391564886</v>
+      </c>
+      <c r="AE30">
+        <v>-0.002384215737684436</v>
+      </c>
+      <c r="AF30">
+        <v>134.0265105079613</v>
+      </c>
     </row>
-    <row r="31" spans="1:29">
+    <row r="31" spans="1:32">
       <c r="A31">
         <v>3</v>
       </c>
       <c r="B31" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C31">
         <v>2018</v>
@@ -3204,13 +3483,22 @@
       <c r="AC31">
         <v>0.09204892667180409</v>
       </c>
+      <c r="AD31">
+        <v>134.075307258832</v>
+      </c>
+      <c r="AE31">
+        <v>0.03348392121249488</v>
+      </c>
+      <c r="AF31">
+        <v>134.0265105079613</v>
+      </c>
     </row>
-    <row r="32" spans="1:29">
+    <row r="32" spans="1:32">
       <c r="A32">
         <v>3</v>
       </c>
       <c r="B32" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C32">
         <v>2019</v>
@@ -3293,13 +3581,22 @@
       <c r="AC32">
         <v>-0.3382930167239859</v>
       </c>
+      <c r="AD32">
+        <v>128.7858066616341</v>
+      </c>
+      <c r="AE32">
+        <v>-0.03945171340899112</v>
+      </c>
+      <c r="AF32">
+        <v>134.0265105079613</v>
+      </c>
     </row>
-    <row r="33" spans="1:29">
+    <row r="33" spans="1:32">
       <c r="A33">
         <v>3</v>
       </c>
       <c r="B33" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C33">
         <v>2020</v>
@@ -3382,13 +3679,22 @@
       <c r="AC33">
         <v>-0.2027455456725192</v>
       </c>
+      <c r="AD33">
+        <v>128.6212754018621</v>
+      </c>
+      <c r="AE33">
+        <v>-0.001277557395779616</v>
+      </c>
+      <c r="AF33">
+        <v>134.0265105079613</v>
+      </c>
     </row>
-    <row r="34" spans="1:29">
+    <row r="34" spans="1:32">
       <c r="A34">
         <v>3</v>
       </c>
       <c r="B34" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C34">
         <v>2021</v>
@@ -3471,13 +3777,22 @@
       <c r="AC34">
         <v>0.6867008742266303</v>
       </c>
+      <c r="AD34">
+        <v>142.6908728185885</v>
+      </c>
+      <c r="AE34">
+        <v>0.1093877927486542</v>
+      </c>
+      <c r="AF34">
+        <v>134.0265105079613</v>
+      </c>
     </row>
-    <row r="35" spans="1:29">
+    <row r="35" spans="1:32">
       <c r="A35">
         <v>4</v>
       </c>
       <c r="B35" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C35">
         <v>2011</v>
@@ -3542,13 +3857,22 @@
       <c r="AC35">
         <v>0.3491587199428436</v>
       </c>
+      <c r="AD35">
+        <v>138.157866352344</v>
+      </c>
+      <c r="AE35">
+        <v>0.1458613604770087</v>
+      </c>
+      <c r="AF35">
+        <v>132.8620301433149</v>
+      </c>
     </row>
-    <row r="36" spans="1:29">
+    <row r="36" spans="1:32">
       <c r="A36">
         <v>4</v>
       </c>
       <c r="B36" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C36">
         <v>2012</v>
@@ -3631,13 +3955,22 @@
       <c r="AC36">
         <v>-0.1379182896681743</v>
       </c>
+      <c r="AD36">
+        <v>135.7739550141928</v>
+      </c>
+      <c r="AE36">
+        <v>-0.01725498084974442</v>
+      </c>
+      <c r="AF36">
+        <v>132.8620301433149</v>
+      </c>
     </row>
-    <row r="37" spans="1:29">
+    <row r="37" spans="1:32">
       <c r="A37">
         <v>4</v>
       </c>
       <c r="B37" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C37">
         <v>2013</v>
@@ -3720,13 +4053,22 @@
       <c r="AC37">
         <v>0.2984701344154055</v>
       </c>
+      <c r="AD37">
+        <v>133.2173040544993</v>
+      </c>
+      <c r="AE37">
+        <v>-0.0188302017086136</v>
+      </c>
+      <c r="AF37">
+        <v>132.8620301433149</v>
+      </c>
     </row>
-    <row r="38" spans="1:29">
+    <row r="38" spans="1:32">
       <c r="A38">
         <v>4</v>
       </c>
       <c r="B38" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C38">
         <v>2014</v>
@@ -3809,13 +4151,22 @@
       <c r="AC38">
         <v>-0.08675589108569781</v>
       </c>
+      <c r="AD38">
+        <v>134.89201336386</v>
+      </c>
+      <c r="AE38">
+        <v>0.01257125957657546</v>
+      </c>
+      <c r="AF38">
+        <v>132.8620301433149</v>
+      </c>
     </row>
-    <row r="39" spans="1:29">
+    <row r="39" spans="1:32">
       <c r="A39">
         <v>4</v>
       </c>
       <c r="B39" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C39">
         <v>2015</v>
@@ -3898,13 +4249,22 @@
       <c r="AC39">
         <v>-0.127859645929598</v>
       </c>
+      <c r="AD39">
+        <v>124.2208291656289</v>
+      </c>
+      <c r="AE39">
+        <v>-0.0791090883153065</v>
+      </c>
+      <c r="AF39">
+        <v>132.8620301433149</v>
+      </c>
     </row>
-    <row r="40" spans="1:29">
+    <row r="40" spans="1:32">
       <c r="A40">
         <v>4</v>
       </c>
       <c r="B40" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C40">
         <v>2016</v>
@@ -3987,13 +4347,22 @@
       <c r="AC40">
         <v>-0.103446182976767</v>
       </c>
+      <c r="AD40">
+        <v>130.4039698280918</v>
+      </c>
+      <c r="AE40">
+        <v>0.04977539357927441</v>
+      </c>
+      <c r="AF40">
+        <v>132.8620301433149</v>
+      </c>
     </row>
-    <row r="41" spans="1:29">
+    <row r="41" spans="1:32">
       <c r="A41">
         <v>4</v>
       </c>
       <c r="B41" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C41">
         <v>2017</v>
@@ -4076,13 +4445,22 @@
       <c r="AC41">
         <v>0.1244640462140472</v>
       </c>
+      <c r="AD41">
+        <v>126.9500033721569</v>
+      </c>
+      <c r="AE41">
+        <v>-0.02648666647563158</v>
+      </c>
+      <c r="AF41">
+        <v>132.8620301433149</v>
+      </c>
     </row>
-    <row r="42" spans="1:29">
+    <row r="42" spans="1:32">
       <c r="A42">
         <v>4</v>
       </c>
       <c r="B42" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C42">
         <v>2018</v>
@@ -4165,13 +4543,22 @@
       <c r="AC42">
         <v>0.2277215519551674</v>
       </c>
+      <c r="AD42">
+        <v>138.4577490588026</v>
+      </c>
+      <c r="AE42">
+        <v>0.09064785648654539</v>
+      </c>
+      <c r="AF42">
+        <v>132.8620301433149</v>
+      </c>
     </row>
-    <row r="43" spans="1:29">
+    <row r="43" spans="1:32">
       <c r="A43">
         <v>4</v>
       </c>
       <c r="B43" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C43">
         <v>2019</v>
@@ -4254,13 +4641,22 @@
       <c r="AC43">
         <v>-0.316645073515244</v>
       </c>
+      <c r="AD43">
+        <v>130.6279426002859</v>
+      </c>
+      <c r="AE43">
+        <v>-0.05655014985973372</v>
+      </c>
+      <c r="AF43">
+        <v>132.8620301433149</v>
+      </c>
     </row>
-    <row r="44" spans="1:29">
+    <row r="44" spans="1:32">
       <c r="A44">
         <v>4</v>
       </c>
       <c r="B44" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C44">
         <v>2020</v>
@@ -4343,13 +4739,22 @@
       <c r="AC44">
         <v>-0.3062742189868776</v>
       </c>
+      <c r="AD44">
+        <v>123.9560548757316</v>
+      </c>
+      <c r="AE44">
+        <v>-0.05107550185468279</v>
+      </c>
+      <c r="AF44">
+        <v>132.8620301433149</v>
+      </c>
     </row>
-    <row r="45" spans="1:29">
+    <row r="45" spans="1:32">
       <c r="A45">
         <v>4</v>
       </c>
       <c r="B45" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C45">
         <v>2021</v>
@@ -4432,13 +4837,22 @@
       <c r="AC45">
         <v>0.6144195399666204</v>
       </c>
+      <c r="AD45">
+        <v>144.8246438908704</v>
+      </c>
+      <c r="AE45">
+        <v>0.1683547369756162</v>
+      </c>
+      <c r="AF45">
+        <v>132.8620301433149</v>
+      </c>
     </row>
-    <row r="46" spans="1:29">
+    <row r="46" spans="1:32">
       <c r="A46">
         <v>5</v>
       </c>
       <c r="B46" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C46">
         <v>2011</v>
@@ -4503,13 +4917,22 @@
       <c r="AC46">
         <v>0.4184271080778834</v>
       </c>
+      <c r="AD46">
+        <v>134.5596839534473</v>
+      </c>
+      <c r="AE46">
+        <v>0.1900065451549404</v>
+      </c>
+      <c r="AF46">
+        <v>131.8336534128878</v>
+      </c>
     </row>
-    <row r="47" spans="1:29">
+    <row r="47" spans="1:32">
       <c r="A47">
         <v>5</v>
       </c>
       <c r="B47" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C47">
         <v>2012</v>
@@ -4592,13 +5015,22 @@
       <c r="AC47">
         <v>-0.07746471133598676</v>
       </c>
+      <c r="AD47">
+        <v>132.5526022082678</v>
+      </c>
+      <c r="AE47">
+        <v>-0.01491592196273228</v>
+      </c>
+      <c r="AF47">
+        <v>131.8336534128878</v>
+      </c>
     </row>
-    <row r="48" spans="1:29">
+    <row r="48" spans="1:32">
       <c r="A48">
         <v>5</v>
       </c>
       <c r="B48" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C48">
         <v>2013</v>
@@ -4681,13 +5113,22 @@
       <c r="AC48">
         <v>0.1738720264539917</v>
       </c>
+      <c r="AD48">
+        <v>131.6435286031115</v>
+      </c>
+      <c r="AE48">
+        <v>-0.006858210174764179</v>
+      </c>
+      <c r="AF48">
+        <v>131.8336534128878</v>
+      </c>
     </row>
-    <row r="49" spans="1:29">
+    <row r="49" spans="1:32">
       <c r="A49">
         <v>5</v>
       </c>
       <c r="B49" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C49">
         <v>2014</v>
@@ -4770,13 +5211,22 @@
       <c r="AC49">
         <v>-0.1780244528582049</v>
       </c>
+      <c r="AD49">
+        <v>138.4614258692378</v>
+      </c>
+      <c r="AE49">
+        <v>0.05179059949601772</v>
+      </c>
+      <c r="AF49">
+        <v>131.8336534128878</v>
+      </c>
     </row>
-    <row r="50" spans="1:29">
+    <row r="50" spans="1:32">
       <c r="A50">
         <v>5</v>
       </c>
       <c r="B50" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C50">
         <v>2015</v>
@@ -4859,13 +5309,22 @@
       <c r="AC50">
         <v>-0.1339844390959359</v>
       </c>
+      <c r="AD50">
+        <v>119.5820938420155</v>
+      </c>
+      <c r="AE50">
+        <v>-0.1363508421836701</v>
+      </c>
+      <c r="AF50">
+        <v>131.8336534128878</v>
+      </c>
     </row>
-    <row r="51" spans="1:29">
+    <row r="51" spans="1:32">
       <c r="A51">
         <v>5</v>
       </c>
       <c r="B51" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C51">
         <v>2016</v>
@@ -4948,13 +5407,22 @@
       <c r="AC51">
         <v>-0.02584965370915671</v>
       </c>
+      <c r="AD51">
+        <v>131.6346640924074</v>
+      </c>
+      <c r="AE51">
+        <v>0.1007890885931053</v>
+      </c>
+      <c r="AF51">
+        <v>131.8336534128878</v>
+      </c>
     </row>
-    <row r="52" spans="1:29">
+    <row r="52" spans="1:32">
       <c r="A52">
         <v>5</v>
       </c>
       <c r="B52" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C52">
         <v>2017</v>
@@ -5037,13 +5505,22 @@
       <c r="AC52">
         <v>0.2443289226745911</v>
       </c>
+      <c r="AD52">
+        <v>126.242693274929</v>
+      </c>
+      <c r="AE52">
+        <v>-0.04096163312798218</v>
+      </c>
+      <c r="AF52">
+        <v>131.8336534128878</v>
+      </c>
     </row>
-    <row r="53" spans="1:29">
+    <row r="53" spans="1:32">
       <c r="A53">
         <v>5</v>
       </c>
       <c r="B53" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C53">
         <v>2018</v>
@@ -5126,13 +5603,22 @@
       <c r="AC53">
         <v>0.06326841586799947</v>
       </c>
+      <c r="AD53">
+        <v>139.460382741722</v>
+      </c>
+      <c r="AE53">
+        <v>0.1047006295881829</v>
+      </c>
+      <c r="AF53">
+        <v>131.8336534128878</v>
+      </c>
     </row>
-    <row r="54" spans="1:29">
+    <row r="54" spans="1:32">
       <c r="A54">
         <v>5</v>
       </c>
       <c r="B54" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C54">
         <v>2019</v>
@@ -5215,13 +5701,22 @@
       <c r="AC54">
         <v>-0.2796544160217044</v>
       </c>
+      <c r="AD54">
+        <v>129.0277848638889</v>
+      </c>
+      <c r="AE54">
+        <v>-0.074806892629529</v>
+      </c>
+      <c r="AF54">
+        <v>131.8336534128878</v>
+      </c>
     </row>
-    <row r="55" spans="1:29">
+    <row r="55" spans="1:32">
       <c r="A55">
         <v>5</v>
       </c>
       <c r="B55" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C55">
         <v>2020</v>
@@ -5304,13 +5799,22 @@
       <c r="AC55">
         <v>-0.3183913330668571</v>
       </c>
+      <c r="AD55">
+        <v>122.4989977428031</v>
+      </c>
+      <c r="AE55">
+        <v>-0.05059985434899184</v>
+      </c>
+      <c r="AF55">
+        <v>131.8336534128878</v>
+      </c>
     </row>
-    <row r="56" spans="1:29">
+    <row r="56" spans="1:32">
       <c r="A56">
         <v>5</v>
       </c>
       <c r="B56" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C56">
         <v>2021</v>
@@ -5393,13 +5897,22 @@
       <c r="AC56">
         <v>0.6238528638744085</v>
       </c>
+      <c r="AD56">
+        <v>144.5063303499352</v>
+      </c>
+      <c r="AE56">
+        <v>0.1796531646188508</v>
+      </c>
+      <c r="AF56">
+        <v>131.8336534128878</v>
+      </c>
     </row>
-    <row r="57" spans="1:29">
+    <row r="57" spans="1:32">
       <c r="A57">
         <v>6</v>
       </c>
       <c r="B57" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C57">
         <v>2011</v>
@@ -5464,13 +5977,22 @@
       <c r="AC57">
         <v>0.3015963108185993</v>
       </c>
+      <c r="AD57">
+        <v>130.8959975586919</v>
+      </c>
+      <c r="AE57">
+        <v>0.1233689959197111</v>
+      </c>
+      <c r="AF57">
+        <v>131.8503426514172</v>
+      </c>
     </row>
-    <row r="58" spans="1:29">
+    <row r="58" spans="1:32">
       <c r="A58">
         <v>6</v>
       </c>
       <c r="B58" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C58">
         <v>2012</v>
@@ -5553,13 +6075,22 @@
       <c r="AC58">
         <v>-0.1000880010943447</v>
       </c>
+      <c r="AD58">
+        <v>133.9923028815652</v>
+      </c>
+      <c r="AE58">
+        <v>0.02365469823846178</v>
+      </c>
+      <c r="AF58">
+        <v>131.8503426514172</v>
+      </c>
     </row>
-    <row r="59" spans="1:29">
+    <row r="59" spans="1:32">
       <c r="A59">
         <v>6</v>
       </c>
       <c r="B59" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C59">
         <v>2013</v>
@@ -5642,13 +6173,22 @@
       <c r="AC59">
         <v>0.1009864651799957</v>
       </c>
+      <c r="AD59">
+        <v>129.3588169657442</v>
+      </c>
+      <c r="AE59">
+        <v>-0.03458023943298083</v>
+      </c>
+      <c r="AF59">
+        <v>131.8503426514172</v>
+      </c>
     </row>
-    <row r="60" spans="1:29">
+    <row r="60" spans="1:32">
       <c r="A60">
         <v>6</v>
       </c>
       <c r="B60" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C60">
         <v>2014</v>
@@ -5731,13 +6271,22 @@
       <c r="AC60">
         <v>-0.1196819557934453</v>
       </c>
+      <c r="AD60">
+        <v>134.6097570740081</v>
+      </c>
+      <c r="AE60">
+        <v>0.04059205419027911</v>
+      </c>
+      <c r="AF60">
+        <v>131.8503426514172</v>
+      </c>
     </row>
-    <row r="61" spans="1:29">
+    <row r="61" spans="1:32">
       <c r="A61">
         <v>6</v>
       </c>
       <c r="B61" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C61">
         <v>2015</v>
@@ -5820,13 +6369,22 @@
       <c r="AC61">
         <v>-0.02406350680923541</v>
       </c>
+      <c r="AD61">
+        <v>121.4161101089869</v>
+      </c>
+      <c r="AE61">
+        <v>-0.09801404632033728</v>
+      </c>
+      <c r="AF61">
+        <v>131.8503426514172</v>
+      </c>
     </row>
-    <row r="62" spans="1:29">
+    <row r="62" spans="1:32">
       <c r="A62">
         <v>6</v>
       </c>
       <c r="B62" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C62">
         <v>2016</v>
@@ -5909,13 +6467,22 @@
       <c r="AC62">
         <v>-0.115767839578338</v>
       </c>
+      <c r="AD62">
+        <v>137.1704195128935</v>
+      </c>
+      <c r="AE62">
+        <v>0.1297546873290951</v>
+      </c>
+      <c r="AF62">
+        <v>131.8503426514172</v>
+      </c>
     </row>
-    <row r="63" spans="1:29">
+    <row r="63" spans="1:32">
       <c r="A63">
         <v>6</v>
       </c>
       <c r="B63" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C63">
         <v>2017</v>
@@ -5998,13 +6565,22 @@
       <c r="AC63">
         <v>0.1687928365290272</v>
       </c>
+      <c r="AD63">
+        <v>127.7268868075617</v>
+      </c>
+      <c r="AE63">
+        <v>-0.06884525642530459</v>
+      </c>
+      <c r="AF63">
+        <v>131.8503426514172</v>
+      </c>
     </row>
-    <row r="64" spans="1:29">
+    <row r="64" spans="1:32">
       <c r="A64">
         <v>6</v>
       </c>
       <c r="B64" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C64">
         <v>2018</v>
@@ -6087,13 +6663,22 @@
       <c r="AC64">
         <v>-0.0741128977856611</v>
       </c>
+      <c r="AD64">
+        <v>134.1222299541411</v>
+      </c>
+      <c r="AE64">
+        <v>0.05007045349985595</v>
+      </c>
+      <c r="AF64">
+        <v>131.8503426514172</v>
+      </c>
     </row>
-    <row r="65" spans="1:29">
+    <row r="65" spans="1:32">
       <c r="A65">
         <v>6</v>
       </c>
       <c r="B65" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C65">
         <v>2019</v>
@@ -6176,13 +6761,22 @@
       <c r="AC65">
         <v>-0.2361514341294483</v>
       </c>
+      <c r="AD65">
+        <v>128.518136827369</v>
+      </c>
+      <c r="AE65">
+        <v>-0.04178347712149033</v>
+      </c>
+      <c r="AF65">
+        <v>131.8503426514172</v>
+      </c>
     </row>
-    <row r="66" spans="1:29">
+    <row r="66" spans="1:32">
       <c r="A66">
         <v>6</v>
       </c>
       <c r="B66" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C66">
         <v>2020</v>
@@ -6265,13 +6859,22 @@
       <c r="AC66">
         <v>-0.2090632688802001</v>
       </c>
+      <c r="AD66">
+        <v>130.727532434294</v>
+      </c>
+      <c r="AE66">
+        <v>0.01719131370456073</v>
+      </c>
+      <c r="AF66">
+        <v>131.8503426514172</v>
+      </c>
     </row>
-    <row r="67" spans="1:29">
+    <row r="67" spans="1:32">
       <c r="A67">
         <v>6</v>
       </c>
       <c r="B67" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C67">
         <v>2021</v>
@@ -6354,13 +6957,22 @@
       <c r="AC67">
         <v>0.790915933034948</v>
       </c>
+      <c r="AD67">
+        <v>141.8155790403333</v>
+      </c>
+      <c r="AE67">
+        <v>0.08481799051483163</v>
+      </c>
+      <c r="AF67">
+        <v>131.8503426514172</v>
+      </c>
     </row>
-    <row r="68" spans="1:29">
+    <row r="68" spans="1:32">
       <c r="A68">
         <v>7</v>
       </c>
       <c r="B68" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C68">
         <v>2011</v>
@@ -6425,13 +7037,22 @@
       <c r="AC68">
         <v>0.2963885650291411</v>
       </c>
+      <c r="AD68">
+        <v>133.6596344429055</v>
+      </c>
+      <c r="AE68">
+        <v>0.1275148751469983</v>
+      </c>
+      <c r="AF68">
+        <v>132.8499118901065</v>
+      </c>
     </row>
-    <row r="69" spans="1:29">
+    <row r="69" spans="1:32">
       <c r="A69">
         <v>7</v>
       </c>
       <c r="B69" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C69">
         <v>2012</v>
@@ -6514,13 +7135,22 @@
       <c r="AC69">
         <v>-0.07489446730170313</v>
       </c>
+      <c r="AD69">
+        <v>140.4742204725378</v>
+      </c>
+      <c r="AE69">
+        <v>0.05098462268010451</v>
+      </c>
+      <c r="AF69">
+        <v>132.8499118901065</v>
+      </c>
     </row>
-    <row r="70" spans="1:29">
+    <row r="70" spans="1:32">
       <c r="A70">
         <v>7</v>
       </c>
       <c r="B70" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C70">
         <v>2013</v>
@@ -6603,13 +7233,22 @@
       <c r="AC70">
         <v>0.101385571332993</v>
       </c>
+      <c r="AD70">
+        <v>136.1071641863124</v>
+      </c>
+      <c r="AE70">
+        <v>-0.03108795529553487</v>
+      </c>
+      <c r="AF70">
+        <v>132.8499118901065</v>
+      </c>
     </row>
-    <row r="71" spans="1:29">
+    <row r="71" spans="1:32">
       <c r="A71">
         <v>7</v>
       </c>
       <c r="B71" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C71">
         <v>2014</v>
@@ -6692,13 +7331,22 @@
       <c r="AC71">
         <v>-0.1206428434428105</v>
       </c>
+      <c r="AD71">
+        <v>130.2037750180781</v>
+      </c>
+      <c r="AE71">
+        <v>-0.04337309651204935</v>
+      </c>
+      <c r="AF71">
+        <v>132.8499118901065</v>
+      </c>
     </row>
-    <row r="72" spans="1:29">
+    <row r="72" spans="1:32">
       <c r="A72">
         <v>7</v>
       </c>
       <c r="B72" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C72">
         <v>2015</v>
@@ -6781,13 +7429,22 @@
       <c r="AC72">
         <v>-0.05606265389994169</v>
       </c>
+      <c r="AD72">
+        <v>120.8795809114708</v>
+      </c>
+      <c r="AE72">
+        <v>-0.07161231773282117</v>
+      </c>
+      <c r="AF72">
+        <v>132.8499118901065</v>
+      </c>
     </row>
-    <row r="73" spans="1:29">
+    <row r="73" spans="1:32">
       <c r="A73">
         <v>7</v>
       </c>
       <c r="B73" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C73">
         <v>2016</v>
@@ -6870,13 +7527,22 @@
       <c r="AC73">
         <v>-0.1866956325367328</v>
       </c>
+      <c r="AD73">
+        <v>136.7541113472318</v>
+      </c>
+      <c r="AE73">
+        <v>0.1313251610905828</v>
+      </c>
+      <c r="AF73">
+        <v>132.8499118901065</v>
+      </c>
     </row>
-    <row r="74" spans="1:29">
+    <row r="74" spans="1:32">
       <c r="A74">
         <v>7</v>
       </c>
       <c r="B74" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C74">
         <v>2017</v>
@@ -6959,13 +7625,22 @@
       <c r="AC74">
         <v>0.2808857617554978</v>
       </c>
+      <c r="AD74">
+        <v>127.0108426496488</v>
+      </c>
+      <c r="AE74">
+        <v>-0.07124662360493095</v>
+      </c>
+      <c r="AF74">
+        <v>132.8499118901065</v>
+      </c>
     </row>
-    <row r="75" spans="1:29">
+    <row r="75" spans="1:32">
       <c r="A75">
         <v>7</v>
       </c>
       <c r="B75" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C75">
         <v>2018</v>
@@ -7048,13 +7723,22 @@
       <c r="AC75">
         <v>0.02311285426485199</v>
       </c>
+      <c r="AD75">
+        <v>133.5721029403324</v>
+      </c>
+      <c r="AE75">
+        <v>0.05165905645380597</v>
+      </c>
+      <c r="AF75">
+        <v>132.8499118901065</v>
+      </c>
     </row>
-    <row r="76" spans="1:29">
+    <row r="76" spans="1:32">
       <c r="A76">
         <v>7</v>
       </c>
       <c r="B76" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C76">
         <v>2019</v>
@@ -7137,13 +7821,22 @@
       <c r="AC76">
         <v>-0.2065707446421599</v>
       </c>
+      <c r="AD76">
+        <v>129.5330092403032</v>
+      </c>
+      <c r="AE76">
+        <v>-0.03023905150189599</v>
+      </c>
+      <c r="AF76">
+        <v>132.8499118901065</v>
+      </c>
     </row>
-    <row r="77" spans="1:29">
+    <row r="77" spans="1:32">
       <c r="A77">
         <v>7</v>
       </c>
       <c r="B77" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C77">
         <v>2020</v>
@@ -7226,13 +7919,22 @@
       <c r="AC77">
         <v>-0.2965178359727726</v>
       </c>
+      <c r="AD77">
+        <v>130.9698062984764</v>
+      </c>
+      <c r="AE77">
+        <v>0.01109213062060288</v>
+      </c>
+      <c r="AF77">
+        <v>132.8499118901065</v>
+      </c>
     </row>
-    <row r="78" spans="1:29">
+    <row r="78" spans="1:32">
       <c r="A78">
         <v>7</v>
       </c>
       <c r="B78" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C78">
         <v>2021</v>
@@ -7315,13 +8017,22 @@
       <c r="AC78">
         <v>0.6562697640810218</v>
       </c>
+      <c r="AD78">
+        <v>142.1847832838741</v>
+      </c>
+      <c r="AE78">
+        <v>0.08563024793546048</v>
+      </c>
+      <c r="AF78">
+        <v>132.8499118901065</v>
+      </c>
     </row>
-    <row r="79" spans="1:29">
+    <row r="79" spans="1:32">
       <c r="A79">
         <v>8</v>
       </c>
       <c r="B79" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C79">
         <v>2011</v>
@@ -7386,13 +8097,22 @@
       <c r="AC79">
         <v>0.43237757690339</v>
       </c>
+      <c r="AD79">
+        <v>136.7930994251751</v>
+      </c>
+      <c r="AE79">
+        <v>0.1140914936579214</v>
+      </c>
+      <c r="AF79">
+        <v>133.5725192805276</v>
+      </c>
     </row>
-    <row r="80" spans="1:29">
+    <row r="80" spans="1:32">
       <c r="A80">
         <v>8</v>
       </c>
       <c r="B80" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C80">
         <v>2012</v>
@@ -7475,13 +8195,22 @@
       <c r="AC80">
         <v>-0.1818038700997001</v>
       </c>
+      <c r="AD80">
+        <v>151.3710697653637</v>
+      </c>
+      <c r="AE80">
+        <v>0.1065694863370112</v>
+      </c>
+      <c r="AF80">
+        <v>133.5725192805276</v>
+      </c>
     </row>
-    <row r="81" spans="1:29">
+    <row r="81" spans="1:32">
       <c r="A81">
         <v>8</v>
       </c>
       <c r="B81" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C81">
         <v>2013</v>
@@ -7564,13 +8293,22 @@
       <c r="AC81">
         <v>0.1270574564848426</v>
       </c>
+      <c r="AD81">
+        <v>128.5257234793937</v>
+      </c>
+      <c r="AE81">
+        <v>-0.1509228039504639</v>
+      </c>
+      <c r="AF81">
+        <v>133.5725192805276</v>
+      </c>
     </row>
-    <row r="82" spans="1:29">
+    <row r="82" spans="1:32">
       <c r="A82">
         <v>8</v>
       </c>
       <c r="B82" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C82">
         <v>2014</v>
@@ -7653,13 +8391,22 @@
       <c r="AC82">
         <v>-0.2020827020267462</v>
       </c>
+      <c r="AD82">
+        <v>131.7992674037326</v>
+      </c>
+      <c r="AE82">
+        <v>0.02546995135074015</v>
+      </c>
+      <c r="AF82">
+        <v>133.5725192805276</v>
+      </c>
     </row>
-    <row r="83" spans="1:29">
+    <row r="83" spans="1:32">
       <c r="A83">
         <v>8</v>
       </c>
       <c r="B83" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C83">
         <v>2015</v>
@@ -7742,13 +8489,22 @@
       <c r="AC83">
         <v>-0.006987698370497286</v>
       </c>
+      <c r="AD83">
+        <v>125.3624172051539</v>
+      </c>
+      <c r="AE83">
+        <v>-0.04883828510867971</v>
+      </c>
+      <c r="AF83">
+        <v>133.5725192805276</v>
+      </c>
     </row>
-    <row r="84" spans="1:29">
+    <row r="84" spans="1:32">
       <c r="A84">
         <v>8</v>
       </c>
       <c r="B84" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C84">
         <v>2016</v>
@@ -7831,13 +8587,22 @@
       <c r="AC84">
         <v>-0.07694202755021107</v>
       </c>
+      <c r="AD84">
+        <v>139.8957725277637</v>
+      </c>
+      <c r="AE84">
+        <v>0.1159307202797955</v>
+      </c>
+      <c r="AF84">
+        <v>133.5725192805276</v>
+      </c>
     </row>
-    <row r="85" spans="1:29">
+    <row r="85" spans="1:32">
       <c r="A85">
         <v>8</v>
       </c>
       <c r="B85" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C85">
         <v>2017</v>
@@ -7920,13 +8685,22 @@
       <c r="AC85">
         <v>0.2209363583731048</v>
       </c>
+      <c r="AD85">
+        <v>126.6005252912394</v>
+      </c>
+      <c r="AE85">
+        <v>-0.09503680487475585</v>
+      </c>
+      <c r="AF85">
+        <v>133.5725192805276</v>
+      </c>
     </row>
-    <row r="86" spans="1:29">
+    <row r="86" spans="1:32">
       <c r="A86">
         <v>8</v>
       </c>
       <c r="B86" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C86">
         <v>2018</v>
@@ -8009,13 +8783,22 @@
       <c r="AC86">
         <v>-0.0003848442984267786</v>
       </c>
+      <c r="AD86">
+        <v>126.6567001720676</v>
+      </c>
+      <c r="AE86">
+        <v>0.0004437175967402229</v>
+      </c>
+      <c r="AF86">
+        <v>133.5725192805276</v>
+      </c>
     </row>
-    <row r="87" spans="1:29">
+    <row r="87" spans="1:32">
       <c r="A87">
         <v>8</v>
       </c>
       <c r="B87" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C87">
         <v>2019</v>
@@ -8098,13 +8881,22 @@
       <c r="AC87">
         <v>-0.3031541925149661</v>
       </c>
+      <c r="AD87">
+        <v>132.2930129861167</v>
+      </c>
+      <c r="AE87">
+        <v>0.0445007078693187</v>
+      </c>
+      <c r="AF87">
+        <v>133.5725192805276</v>
+      </c>
     </row>
-    <row r="88" spans="1:29">
+    <row r="88" spans="1:32">
       <c r="A88">
         <v>8</v>
       </c>
       <c r="B88" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C88">
         <v>2020</v>
@@ -8187,13 +8979,22 @@
       <c r="AC88">
         <v>-0.2026957055939365</v>
       </c>
+      <c r="AD88">
+        <v>131.5280777123958</v>
+      </c>
+      <c r="AE88">
+        <v>-0.005782129051677187</v>
+      </c>
+      <c r="AF88">
+        <v>133.5725192805276</v>
+      </c>
     </row>
-    <row r="89" spans="1:29">
+    <row r="89" spans="1:32">
       <c r="A89">
         <v>8</v>
       </c>
       <c r="B89" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C89">
         <v>2021</v>
@@ -8276,13 +9077,22 @@
       <c r="AC89">
         <v>0.6400493272717882</v>
       </c>
+      <c r="AD89">
+        <v>138.4720461174012</v>
+      </c>
+      <c r="AE89">
+        <v>0.0527945707546138</v>
+      </c>
+      <c r="AF89">
+        <v>133.5725192805276</v>
+      </c>
     </row>
-    <row r="90" spans="1:29">
+    <row r="90" spans="1:32">
       <c r="A90">
         <v>9</v>
       </c>
       <c r="B90" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C90">
         <v>2011</v>
@@ -8347,13 +9157,22 @@
       <c r="AC90">
         <v>0.2907233066130119</v>
       </c>
+      <c r="AD90">
+        <v>141.5956170161337</v>
+      </c>
+      <c r="AE90">
+        <v>0.131603858475458</v>
+      </c>
+      <c r="AF90">
+        <v>136.9988585955319</v>
+      </c>
     </row>
-    <row r="91" spans="1:29">
+    <row r="91" spans="1:32">
       <c r="A91">
         <v>9</v>
       </c>
       <c r="B91" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C91">
         <v>2012</v>
@@ -8436,13 +9255,22 @@
       <c r="AC91">
         <v>-0.1500884366902923</v>
       </c>
+      <c r="AD91">
+        <v>151.6206285124406</v>
+      </c>
+      <c r="AE91">
+        <v>0.07080029528855203</v>
+      </c>
+      <c r="AF91">
+        <v>136.9988585955319</v>
+      </c>
     </row>
-    <row r="92" spans="1:29">
+    <row r="92" spans="1:32">
       <c r="A92">
         <v>9</v>
       </c>
       <c r="B92" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C92">
         <v>2013</v>
@@ -8525,13 +9353,22 @@
       <c r="AC92">
         <v>0.02977216008999362</v>
       </c>
+      <c r="AD92">
+        <v>141.1292563979021</v>
+      </c>
+      <c r="AE92">
+        <v>-0.06919488606181123</v>
+      </c>
+      <c r="AF92">
+        <v>136.9988585955319</v>
+      </c>
     </row>
-    <row r="93" spans="1:29">
+    <row r="93" spans="1:32">
       <c r="A93">
         <v>9</v>
       </c>
       <c r="B93" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C93">
         <v>2014</v>
@@ -8614,13 +9451,22 @@
       <c r="AC93">
         <v>-0.06383297043817127</v>
       </c>
+      <c r="AD93">
+        <v>133.5976540528878</v>
+      </c>
+      <c r="AE93">
+        <v>-0.05336669757388635</v>
+      </c>
+      <c r="AF93">
+        <v>136.9988585955319</v>
+      </c>
     </row>
-    <row r="94" spans="1:29">
+    <row r="94" spans="1:32">
       <c r="A94">
         <v>9</v>
       </c>
       <c r="B94" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C94">
         <v>2015</v>
@@ -8703,13 +9549,22 @@
       <c r="AC94">
         <v>-0.02781672981092831</v>
       </c>
+      <c r="AD94">
+        <v>132.0804338456402</v>
+      </c>
+      <c r="AE94">
+        <v>-0.01135663809371201</v>
+      </c>
+      <c r="AF94">
+        <v>136.9988585955319</v>
+      </c>
     </row>
-    <row r="95" spans="1:29">
+    <row r="95" spans="1:32">
       <c r="A95">
         <v>9</v>
       </c>
       <c r="B95" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C95">
         <v>2016</v>
@@ -8792,13 +9647,22 @@
       <c r="AC95">
         <v>-0.1358942760388734</v>
       </c>
+      <c r="AD95">
+        <v>141.8280656503174</v>
+      </c>
+      <c r="AE95">
+        <v>0.07380072521618919</v>
+      </c>
+      <c r="AF95">
+        <v>136.9988585955319</v>
+      </c>
     </row>
-    <row r="96" spans="1:29">
+    <row r="96" spans="1:32">
       <c r="A96">
         <v>9</v>
       </c>
       <c r="B96" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C96">
         <v>2017</v>
@@ -8881,13 +9745,22 @@
       <c r="AC96">
         <v>0.2587699626658282</v>
       </c>
+      <c r="AD96">
+        <v>130.5339215523102</v>
+      </c>
+      <c r="AE96">
+        <v>-0.07963264567009853</v>
+      </c>
+      <c r="AF96">
+        <v>136.9988585955319</v>
+      </c>
     </row>
-    <row r="97" spans="1:29">
+    <row r="97" spans="1:32">
       <c r="A97">
         <v>9</v>
       </c>
       <c r="B97" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C97">
         <v>2018</v>
@@ -8970,13 +9843,22 @@
       <c r="AC97">
         <v>-0.2125199647151436</v>
       </c>
+      <c r="AD97">
+        <v>129.0885487303606</v>
+      </c>
+      <c r="AE97">
+        <v>-0.01107277560316289</v>
+      </c>
+      <c r="AF97">
+        <v>136.9988585955319</v>
+      </c>
     </row>
-    <row r="98" spans="1:29">
+    <row r="98" spans="1:32">
       <c r="A98">
         <v>9</v>
       </c>
       <c r="B98" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C98">
         <v>2019</v>
@@ -9059,13 +9941,22 @@
       <c r="AC98">
         <v>-0.1485148005582401</v>
       </c>
+      <c r="AD98">
+        <v>131.0584656951243</v>
+      </c>
+      <c r="AE98">
+        <v>0.01526019917443255</v>
+      </c>
+      <c r="AF98">
+        <v>136.9988585955319</v>
+      </c>
     </row>
-    <row r="99" spans="1:29">
+    <row r="99" spans="1:32">
       <c r="A99">
         <v>9</v>
       </c>
       <c r="B99" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C99">
         <v>2020</v>
@@ -9148,13 +10039,22 @@
       <c r="AC99">
         <v>0.03174766368908055</v>
       </c>
+      <c r="AD99">
+        <v>131.062744684111</v>
+      </c>
+      <c r="AE99">
+        <v>3.264946651126976E-05</v>
+      </c>
+      <c r="AF99">
+        <v>136.9988585955319</v>
+      </c>
     </row>
-    <row r="100" spans="1:29">
+    <row r="100" spans="1:32">
       <c r="A100">
         <v>9</v>
       </c>
       <c r="B100" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C100">
         <v>2021</v>
@@ -9237,13 +10137,22 @@
       <c r="AC100">
         <v>0.4254517923881449</v>
       </c>
+      <c r="AD100">
+        <v>143.3921084136225</v>
+      </c>
+      <c r="AE100">
+        <v>0.09407222288246597</v>
+      </c>
+      <c r="AF100">
+        <v>136.9988585955319</v>
+      </c>
     </row>
-    <row r="101" spans="1:29">
+    <row r="101" spans="1:32">
       <c r="A101">
         <v>10</v>
       </c>
       <c r="B101" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C101">
         <v>2011</v>
@@ -9308,13 +10217,22 @@
       <c r="AC101">
         <v>0.2731147927679278</v>
       </c>
+      <c r="AD101">
+        <v>144.576928409329</v>
+      </c>
+      <c r="AE101">
+        <v>0.09074212267900927</v>
+      </c>
+      <c r="AF101">
+        <v>137.5244855240853</v>
+      </c>
     </row>
-    <row r="102" spans="1:29">
+    <row r="102" spans="1:32">
       <c r="A102">
         <v>10</v>
       </c>
       <c r="B102" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C102">
         <v>2012</v>
@@ -9397,13 +10315,22 @@
       <c r="AC102">
         <v>-0.007361976775885459</v>
       </c>
+      <c r="AD102">
+        <v>154.2326856262545</v>
+      </c>
+      <c r="AE102">
+        <v>0.06678629379639256</v>
+      </c>
+      <c r="AF102">
+        <v>137.5244855240853</v>
+      </c>
     </row>
-    <row r="103" spans="1:29">
+    <row r="103" spans="1:32">
       <c r="A103">
         <v>10</v>
       </c>
       <c r="B103" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C103">
         <v>2013</v>
@@ -9486,13 +10413,22 @@
       <c r="AC103">
         <v>0.0917985250435589</v>
       </c>
+      <c r="AD103">
+        <v>135.2599806857932</v>
+      </c>
+      <c r="AE103">
+        <v>-0.1230135159964534</v>
+      </c>
+      <c r="AF103">
+        <v>137.5244855240853</v>
+      </c>
     </row>
-    <row r="104" spans="1:29">
+    <row r="104" spans="1:32">
       <c r="A104">
         <v>10</v>
       </c>
       <c r="B104" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C104">
         <v>2014</v>
@@ -9575,13 +10511,22 @@
       <c r="AC104">
         <v>-0.1956798494445465</v>
       </c>
+      <c r="AD104">
+        <v>127.2137635816511</v>
+      </c>
+      <c r="AE104">
+        <v>-0.05948704903953328</v>
+      </c>
+      <c r="AF104">
+        <v>137.5244855240853</v>
+      </c>
     </row>
-    <row r="105" spans="1:29">
+    <row r="105" spans="1:32">
       <c r="A105">
         <v>10</v>
       </c>
       <c r="B105" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C105">
         <v>2015</v>
@@ -9664,13 +10609,22 @@
       <c r="AC105">
         <v>-0.07940624716081257</v>
       </c>
+      <c r="AD105">
+        <v>129.8192613120931</v>
+      </c>
+      <c r="AE105">
+        <v>0.02048125656442523</v>
+      </c>
+      <c r="AF105">
+        <v>137.5244855240853</v>
+      </c>
     </row>
-    <row r="106" spans="1:29">
+    <row r="106" spans="1:32">
       <c r="A106">
         <v>10</v>
       </c>
       <c r="B106" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C106">
         <v>2016</v>
@@ -9753,13 +10707,22 @@
       <c r="AC106">
         <v>-0.05437873557340045</v>
       </c>
+      <c r="AD106">
+        <v>140.3134868838974</v>
+      </c>
+      <c r="AE106">
+        <v>0.08083719985569493</v>
+      </c>
+      <c r="AF106">
+        <v>137.5244855240853</v>
+      </c>
     </row>
-    <row r="107" spans="1:29">
+    <row r="107" spans="1:32">
       <c r="A107">
         <v>10</v>
       </c>
       <c r="B107" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C107">
         <v>2017</v>
@@ -9842,13 +10805,22 @@
       <c r="AC107">
         <v>0.2981836149879311</v>
       </c>
+      <c r="AD107">
+        <v>135.9137607256569</v>
+      </c>
+      <c r="AE107">
+        <v>-0.03135640240970583</v>
+      </c>
+      <c r="AF107">
+        <v>137.5244855240853</v>
+      </c>
     </row>
-    <row r="108" spans="1:29">
+    <row r="108" spans="1:32">
       <c r="A108">
         <v>10</v>
       </c>
       <c r="B108" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C108">
         <v>2018</v>
@@ -9931,13 +10903,22 @@
       <c r="AC108">
         <v>-0.1829015727290243</v>
       </c>
+      <c r="AD108">
+        <v>126.1705216048887</v>
+      </c>
+      <c r="AE108">
+        <v>-0.07168692168289781</v>
+      </c>
+      <c r="AF108">
+        <v>137.5244855240853</v>
+      </c>
     </row>
-    <row r="109" spans="1:29">
+    <row r="109" spans="1:32">
       <c r="A109">
         <v>10</v>
       </c>
       <c r="B109" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C109">
         <v>2019</v>
@@ -10020,13 +11001,22 @@
       <c r="AC109">
         <v>-0.1876512033156399</v>
       </c>
+      <c r="AD109">
+        <v>137.3388439002599</v>
+      </c>
+      <c r="AE109">
+        <v>0.08851768347558697</v>
+      </c>
+      <c r="AF109">
+        <v>137.5244855240853</v>
+      </c>
     </row>
-    <row r="110" spans="1:29">
+    <row r="110" spans="1:32">
       <c r="A110">
         <v>10</v>
       </c>
       <c r="B110" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C110">
         <v>2020</v>
@@ -10109,13 +11099,22 @@
       <c r="AC110">
         <v>-0.02838560607981511</v>
       </c>
+      <c r="AD110">
+        <v>135.7920002973633</v>
+      </c>
+      <c r="AE110">
+        <v>-0.01126297236068197</v>
+      </c>
+      <c r="AF110">
+        <v>137.5244855240853</v>
+      </c>
     </row>
-    <row r="111" spans="1:29">
+    <row r="111" spans="1:32">
       <c r="A111">
         <v>10</v>
       </c>
       <c r="B111" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C111">
         <v>2021</v>
@@ -10198,13 +11197,22 @@
       <c r="AC111">
         <v>0.310353232363539</v>
       </c>
+      <c r="AD111">
+        <v>146.1381077377518</v>
+      </c>
+      <c r="AE111">
+        <v>0.07619084642491591</v>
+      </c>
+      <c r="AF111">
+        <v>137.5244855240853</v>
+      </c>
     </row>
-    <row r="112" spans="1:29">
+    <row r="112" spans="1:32">
       <c r="A112">
         <v>11</v>
       </c>
       <c r="B112" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C112">
         <v>2011</v>
@@ -10269,13 +11277,22 @@
       <c r="AC112">
         <v>0.1173445618369369</v>
       </c>
+      <c r="AD112">
+        <v>144.2657632060383</v>
+      </c>
+      <c r="AE112">
+        <v>0.05399256572219691</v>
+      </c>
+      <c r="AF112">
+        <v>136.2745831499826</v>
+      </c>
     </row>
-    <row r="113" spans="1:29">
+    <row r="113" spans="1:32">
       <c r="A113">
         <v>11</v>
       </c>
       <c r="B113" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C113">
         <v>2012</v>
@@ -10358,13 +11375,22 @@
       <c r="AC113">
         <v>-0.07227981116636129</v>
       </c>
+      <c r="AD113">
+        <v>152.5899808655232</v>
+      </c>
+      <c r="AE113">
+        <v>0.05770057617618085</v>
+      </c>
+      <c r="AF113">
+        <v>136.2745831499826</v>
+      </c>
     </row>
-    <row r="114" spans="1:29">
+    <row r="114" spans="1:32">
       <c r="A114">
         <v>11</v>
       </c>
       <c r="B114" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C114">
         <v>2013</v>
@@ -10447,13 +11473,22 @@
       <c r="AC114">
         <v>0.0540147245298197</v>
       </c>
+      <c r="AD114">
+        <v>136.4136783019794</v>
+      </c>
+      <c r="AE114">
+        <v>-0.1060115642703956</v>
+      </c>
+      <c r="AF114">
+        <v>136.2745831499826</v>
+      </c>
     </row>
-    <row r="115" spans="1:29">
+    <row r="115" spans="1:32">
       <c r="A115">
         <v>11</v>
       </c>
       <c r="B115" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C115">
         <v>2014</v>
@@ -10536,13 +11571,22 @@
       <c r="AC115">
         <v>-0.2364977218524222</v>
       </c>
+      <c r="AD115">
+        <v>126.9644956010252</v>
+      </c>
+      <c r="AE115">
+        <v>-0.06926858668847291</v>
+      </c>
+      <c r="AF115">
+        <v>136.2745831499826</v>
+      </c>
     </row>
-    <row r="116" spans="1:29">
+    <row r="116" spans="1:32">
       <c r="A116">
         <v>11</v>
       </c>
       <c r="B116" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C116">
         <v>2015</v>
@@ -10625,13 +11669,22 @@
       <c r="AC116">
         <v>0.01044449515280821</v>
       </c>
+      <c r="AD116">
+        <v>130.3402910779215</v>
+      </c>
+      <c r="AE116">
+        <v>0.02658849988664835</v>
+      </c>
+      <c r="AF116">
+        <v>136.2745831499826</v>
+      </c>
     </row>
-    <row r="117" spans="1:29">
+    <row r="117" spans="1:32">
       <c r="A117">
         <v>11</v>
       </c>
       <c r="B117" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C117">
         <v>2016</v>
@@ -10714,13 +11767,22 @@
       <c r="AC117">
         <v>0.005018285677688583</v>
       </c>
+      <c r="AD117">
+        <v>135.7670159617564</v>
+      </c>
+      <c r="AE117">
+        <v>0.04163505266833178</v>
+      </c>
+      <c r="AF117">
+        <v>136.2745831499826</v>
+      </c>
     </row>
-    <row r="118" spans="1:29">
+    <row r="118" spans="1:32">
       <c r="A118">
         <v>11</v>
       </c>
       <c r="B118" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C118">
         <v>2017</v>
@@ -10803,13 +11865,22 @@
       <c r="AC118">
         <v>0.3049306530313447</v>
       </c>
+      <c r="AD118">
+        <v>136.8179240852982</v>
+      </c>
+      <c r="AE118">
+        <v>0.007740526048224616</v>
+      </c>
+      <c r="AF118">
+        <v>136.2745831499826</v>
+      </c>
     </row>
-    <row r="119" spans="1:29">
+    <row r="119" spans="1:32">
       <c r="A119">
         <v>11</v>
       </c>
       <c r="B119" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C119">
         <v>2018</v>
@@ -10892,13 +11963,22 @@
       <c r="AC119">
         <v>-0.2921054639704014</v>
       </c>
+      <c r="AD119">
+        <v>126.9081252932563</v>
+      </c>
+      <c r="AE119">
+        <v>-0.07243055950668931</v>
+      </c>
+      <c r="AF119">
+        <v>136.2745831499826</v>
+      </c>
     </row>
-    <row r="120" spans="1:29">
+    <row r="120" spans="1:32">
       <c r="A120">
         <v>11</v>
       </c>
       <c r="B120" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C120">
         <v>2019</v>
@@ -10981,13 +12061,22 @@
       <c r="AC120">
         <v>-0.2187319122304725</v>
       </c>
+      <c r="AD120">
+        <v>130.3216224122787</v>
+      </c>
+      <c r="AE120">
+        <v>0.02689738825732868</v>
+      </c>
+      <c r="AF120">
+        <v>136.2745831499826</v>
+      </c>
     </row>
-    <row r="121" spans="1:29">
+    <row r="121" spans="1:32">
       <c r="A121">
         <v>11</v>
       </c>
       <c r="B121" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C121">
         <v>2020</v>
@@ -11070,13 +12159,22 @@
       <c r="AC121">
         <v>0.2071399702405163</v>
       </c>
+      <c r="AD121">
+        <v>138.2110303772799</v>
+      </c>
+      <c r="AE121">
+        <v>0.06053798148739009</v>
+      </c>
+      <c r="AF121">
+        <v>136.2745831499826</v>
+      </c>
     </row>
-    <row r="122" spans="1:29">
+    <row r="122" spans="1:32">
       <c r="A122">
         <v>11</v>
       </c>
       <c r="B122" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C122">
         <v>2021</v>
@@ -11159,13 +12257,22 @@
       <c r="AC122">
         <v>0.4015497709303537</v>
       </c>
+      <c r="AD122">
+        <v>140.4204874674513</v>
+      </c>
+      <c r="AE122">
+        <v>0.01598611257104565</v>
+      </c>
+      <c r="AF122">
+        <v>136.2745831499826</v>
+      </c>
     </row>
-    <row r="123" spans="1:29">
+    <row r="123" spans="1:32">
       <c r="A123">
         <v>12</v>
       </c>
       <c r="B123" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C123">
         <v>2011</v>
@@ -11230,13 +12337,22 @@
       <c r="AC123">
         <v>0.1110926797345084</v>
       </c>
+      <c r="AD123">
+        <v>141.410877662712</v>
+      </c>
+      <c r="AE123">
+        <v>0.03708822165527437</v>
+      </c>
+      <c r="AF123">
+        <v>134.6294600499599</v>
+      </c>
     </row>
-    <row r="124" spans="1:29">
+    <row r="124" spans="1:32">
       <c r="A124">
         <v>12</v>
       </c>
       <c r="B124" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C124">
         <v>2012</v>
@@ -11319,13 +12435,22 @@
       <c r="AC124">
         <v>-0.09200566444494207</v>
       </c>
+      <c r="AD124">
+        <v>147.1807742037649</v>
+      </c>
+      <c r="AE124">
+        <v>0.04080235294780588</v>
+      </c>
+      <c r="AF124">
+        <v>134.6294600499599</v>
+      </c>
     </row>
-    <row r="125" spans="1:29">
+    <row r="125" spans="1:32">
       <c r="A125">
         <v>12</v>
       </c>
       <c r="B125" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C125">
         <v>2013</v>
@@ -11408,13 +12533,22 @@
       <c r="AC125">
         <v>-0.004566488671456814</v>
       </c>
+      <c r="AD125">
+        <v>129.2389566991934</v>
+      </c>
+      <c r="AE125">
+        <v>-0.1219032689672632</v>
+      </c>
+      <c r="AF125">
+        <v>134.6294600499599</v>
+      </c>
     </row>
-    <row r="126" spans="1:29">
+    <row r="126" spans="1:32">
       <c r="A126">
         <v>12</v>
       </c>
       <c r="B126" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C126">
         <v>2014</v>
@@ -11497,13 +12631,22 @@
       <c r="AC126">
         <v>-0.2053481059795229</v>
       </c>
+      <c r="AD126">
+        <v>127.6034681503818</v>
+      </c>
+      <c r="AE126">
+        <v>-0.01265476440372548</v>
+      </c>
+      <c r="AF126">
+        <v>134.6294600499599</v>
+      </c>
     </row>
-    <row r="127" spans="1:29">
+    <row r="127" spans="1:32">
       <c r="A127">
         <v>12</v>
       </c>
       <c r="B127" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C127">
         <v>2015</v>
@@ -11586,13 +12729,22 @@
       <c r="AC127">
         <v>0.02406365959104861</v>
       </c>
+      <c r="AD127">
+        <v>126.9880415966722</v>
+      </c>
+      <c r="AE127">
+        <v>-0.004822961026296646</v>
+      </c>
+      <c r="AF127">
+        <v>134.6294600499599</v>
+      </c>
     </row>
-    <row r="128" spans="1:29">
+    <row r="128" spans="1:32">
       <c r="A128">
         <v>12</v>
       </c>
       <c r="B128" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C128">
         <v>2016</v>
@@ -11675,13 +12827,22 @@
       <c r="AC128">
         <v>0.04334464401082339</v>
       </c>
+      <c r="AD128">
+        <v>129.5669416886971</v>
+      </c>
+      <c r="AE128">
+        <v>0.02030821217178702</v>
+      </c>
+      <c r="AF128">
+        <v>134.6294600499599</v>
+      </c>
     </row>
-    <row r="129" spans="1:29">
+    <row r="129" spans="1:32">
       <c r="A129">
         <v>12</v>
       </c>
       <c r="B129" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C129">
         <v>2017</v>
@@ -11764,13 +12925,22 @@
       <c r="AC129">
         <v>0.1678323515325071</v>
       </c>
+      <c r="AD129">
+        <v>134.2964736527875</v>
+      </c>
+      <c r="AE129">
+        <v>0.03650261326267712</v>
+      </c>
+      <c r="AF129">
+        <v>134.6294600499599</v>
+      </c>
     </row>
-    <row r="130" spans="1:29">
+    <row r="130" spans="1:32">
       <c r="A130">
         <v>12</v>
       </c>
       <c r="B130" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C130">
         <v>2018</v>
@@ -11853,13 +13023,22 @@
       <c r="AC130">
         <v>-0.2700477428706514</v>
       </c>
+      <c r="AD130">
+        <v>127.0313434770258</v>
+      </c>
+      <c r="AE130">
+        <v>-0.0540976987567453</v>
+      </c>
+      <c r="AF130">
+        <v>134.6294600499599</v>
+      </c>
     </row>
-    <row r="131" spans="1:29">
+    <row r="131" spans="1:32">
       <c r="A131">
         <v>12</v>
       </c>
       <c r="B131" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C131">
         <v>2019</v>
@@ -11942,13 +13121,22 @@
       <c r="AC131">
         <v>-0.2001107856869041</v>
       </c>
+      <c r="AD131">
+        <v>133.0569145434906</v>
+      </c>
+      <c r="AE131">
+        <v>0.04743373486839153</v>
+      </c>
+      <c r="AF131">
+        <v>134.6294600499599</v>
+      </c>
     </row>
-    <row r="132" spans="1:29">
+    <row r="132" spans="1:32">
       <c r="A132">
         <v>12</v>
       </c>
       <c r="B132" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C132">
         <v>2020</v>
@@ -12031,13 +13219,22 @@
       <c r="AC132">
         <v>0.2473222568624713</v>
       </c>
+      <c r="AD132">
+        <v>138.2965350788341</v>
+      </c>
+      <c r="AE132">
+        <v>0.03937879179988713</v>
+      </c>
+      <c r="AF132">
+        <v>134.6294600499599</v>
+      </c>
     </row>
-    <row r="133" spans="1:29">
+    <row r="133" spans="1:32">
       <c r="A133">
         <v>12</v>
       </c>
       <c r="B133" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C133">
         <v>2021</v>
@@ -12119,6 +13316,15 @@
       </c>
       <c r="AC133">
         <v>0.5905395464668235</v>
+      </c>
+      <c r="AD133">
+        <v>146.253733796</v>
+      </c>
+      <c r="AE133">
+        <v>0.05753722399935723</v>
+      </c>
+      <c r="AF133">
+        <v>134.6294600499599</v>
       </c>
     </row>
   </sheetData>

</xml_diff>